<commit_message>
Updated file with BCBB python seminars
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E201CA8-6342-6443-AD57-E0A745B6AA01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E78F5C6-B4EA-C94C-A042-D2D0648E5694}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17600" yWindow="460" windowWidth="33600" windowHeight="25380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="98">
   <si>
     <t>type</t>
   </si>
@@ -241,6 +241,130 @@
   </si>
   <si>
     <t>computational data analysis,epigenetics sequencing</t>
+  </si>
+  <si>
+    <t>Intermediate Python Programming and Best Practices</t>
+  </si>
+  <si>
+    <t>NIH Main Campus, Building 12, Room B51</t>
+  </si>
+  <si>
+    <t>Bioinformatics Programming with Python</t>
+  </si>
+  <si>
+    <t>Building Workflows with Python</t>
+  </si>
+  <si>
+    <t>Biomedical Data Storage and Retrieval (using SQL &amp; NoSQL)</t>
+  </si>
+  <si>
+    <t>Becoming a Reproducible Scientist (Part 1)</t>
+  </si>
+  <si>
+    <t>Becoming a Reproducible Scientist (Part 2)</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>We will explore reasons for reproducible science and delve into practical exercises that will allow you to enhance your data analysis with good, better, and best practices. Topics include introduction to Jupyter Notebook, basic intro to the python programming language, data and project organization, data exploration, automation, publishing, and sharing. This seminar will condense the Data Carpentry Reproducible Science Jupyter workshop held in Berkeley, CA in 2017 &amp; 2018 (https://github.com/Reproducible-Science-Curriculum). Students will receive a Jupyter Notebook with all steps taught in the class for further study and practice. 
+This seminar will be concurrently webcast for those who cannot attend in person (Register here: http://bit.ly/nih-python-register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We will explore reasons for reproducible science and delve into practical exercises that will allow you to enhance your data analysis with good, better, and best practices. Topics include introduction to Jupyter Notebook, basic intro to the python programming language, data and project organization, data exploration, automation, publishing, and sharing. This seminar will condense the Data Carpentry Reproducible Science Jupyter workshop held in Berkeley, CA in 2017 &amp; 2018 (https://github.com/Reproducible-Science-Curriculum). Students will receive a Jupyter Notebook with all steps taught in the class for further study and practice. 
+This seminar will be concurrently webcast for those who cannot attend in person (Register here: http://bit.ly/nih-python-register) </t>
+  </si>
+  <si>
+    <t>reproducibility</t>
+  </si>
+  <si>
+    <t>https://training.cit.nih.gov/class_details.aspx?cId=NIHCIT-SS499</t>
+  </si>
+  <si>
+    <t>https://training.cit.nih.gov/class_details.aspx?cId=NIHCIT-SS500</t>
+  </si>
+  <si>
+    <t>Now that you know the basics of the python programming language, let's take the language to the next level. In the seminar, we will explore some advanced features of the python programming language and we will also explore some best practices to make the best use of the python programming language. Students will receive a Jupyter Notebook with all steps taught in the class for further study and practice. 
+This seminar will be concurrently webcast for those who cannot attend in person (Register here: http://bit.ly/nih-python-register) 
+Prerequisites
+- Introduction to the Command Line webinar (http://bioinformatics.niaid.nih.gov)
+- Introduction to Jupiter notebook
+- Introduction to Programming (with Python) or previous programming experience required</t>
+  </si>
+  <si>
+    <t>python,Jupyter notebook</t>
+  </si>
+  <si>
+    <t>https://training.cit.nih.gov/class_details.aspx?cId=NIHCIT-SS460</t>
+  </si>
+  <si>
+    <t>In this seminar, we will explore the bioinformatics capabilities of the python programming language. We will examine some of the many capabilities of the biopython package as well as delve into the bioconda project for easy bioinformatics software installation. Students will receive a Jupyter Notebook with all steps taught in the class for further study and practice. 
+This seminar will be concurrently webcast for those who cannot attend in person (Register here: http://bit.ly/nih-python-register) 
+Prerequisites
+- Introduction to the Command Line webinar (http://bioinformatics.niaid.nih.gov)
+- Introduction to Jupiter notebook
+- Introduction to Programming (with Python) or previous programming experience required</t>
+  </si>
+  <si>
+    <t>https://training.cit.nih.gov/class_details.aspx?cId=NIHCIT-SS470</t>
+  </si>
+  <si>
+    <t>In this seminar, we will assemble a working pipeline based upon the steps we have learned in the previous seminars while surveying a few methods for building workflows, including the snakemake package. Students will receive a Jupyter Notebook with all steps taught in the class for further study and practice. 
+This seminar will be concurrently webcast for those who cannot attend in person (Register here: http://bit.ly/nih-python-register) 
+Prerequisites
+- Introduction to the Command Line webinar (http://bioinformatics.niaid.nih.gov)
+- Introduction to Jupiter notebook
+- Introduction to Programming (with Python) or previous programming experience required</t>
+  </si>
+  <si>
+    <t>Biological data continues to grow at an incredible rate! In the seminar, we will examine data storage and retrieval strategies, use cases, and practical examples using databases (including MySQL and MongoDB) as well as programming languages to access them (SQL and NoSQL). Programming will be done using the Python programming language. Students will receive a Jupyter Notebook with all steps taught in the class for further study and practice. 
+This seminar will be concurrently webcast for those who cannot attend in person (Register here: http://bit.ly/nih-python-register) 
+Prerequisites
+- Experience with a computer and web browser
+- Familiarity with the Python programming language</t>
+  </si>
+  <si>
+    <t>data storage, MySQL,MongoDB,Jupyter notebook</t>
+  </si>
+  <si>
+    <t>https://training.cit.nih.gov/class_details.aspx?cId=NIHCIT-SS497</t>
+  </si>
+  <si>
+    <t>https://training.cit.nih.gov/class_details.aspx?cId=NIHCIT-SS451</t>
+  </si>
+  <si>
+    <t>https://register.gotowebinar.com/register/2903823797545605121</t>
+  </si>
+  <si>
+    <t>**This event is for NIH Staff only**
+METAGENOTE refers to the collection of metadata from genomics studies using a web-based notebook. METAGENOTE facilitates the annotation of datasets to ensure that metadata is stored in one centralized location for each group and automates the submission of files to the SRA. This tool, developed by NIAID, is freely accessible to all NIH researchers. 
+The webinar will cover easy ways to annotate your samples and submit them to the NCBI Sequence Read Archive (SRA) using METAGENOTE. 
+By attending this webinar, you can expect to learn:
+• What is METAGENOTE and why do I want to use it? 
+• How do I import metadata from Excel files? 
+• How do I share annotated sample group tables with lab members? 
+• How do I submit my sample data to the SRA database automatically?</t>
+  </si>
+  <si>
+    <t>genomic data,SRA</t>
+  </si>
+  <si>
+    <t>Introduction to METAGENOTE</t>
+  </si>
+  <si>
+    <t>GoToWebinar</t>
+  </si>
+  <si>
+    <t>Probes of Dendritic Cell Lectins</t>
+  </si>
+  <si>
+    <t>NCI-Frederick Fort Detrick campus, Bldg. 376, Room 121</t>
+  </si>
+  <si>
+    <t>NCI at Frederick is pleased to announce a forthcoming seminar in the "Molecular Discovery Seminar Series (MDSS)."  The presenter will be Prof. Laura L. Kiessling*, Massachusetts Institute of Technology (MIT), Dept. of Chemistry, Cambridge, MA.
+Prof. Kiessling's talk is entitled "Probes of Dendritic Cell Lectins".
+The seminar will begin at 10:00 a.m. on Thursday, November 8, 2018, at NCI-Frederick in Bldg. 376, Room 121 on the Fort Detrick campus, Frederick, MD.   It will also be video-conferenced 'live' to Building 3, Room 2E04 on the Bethesda campus and Room E-1201 at the Advanced Technology Research Facility (ATRF).
+You will find Prof. Kiessling's bibliography at: https://ncifrederick.cancer.gov/ScientificLibrary/Bibliography/Default.aspx</t>
   </si>
 </sst>
 </file>
@@ -659,11 +783,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -981,7 +1105,7 @@
         <v>43398</v>
       </c>
       <c r="E9" s="11">
-        <f t="shared" ref="E9:E11" si="2">(C9-DATE(1970,1,1))*86400</f>
+        <f t="shared" ref="E9:E19" si="2">(C9-DATE(1970,1,1))*86400</f>
         <v>1540425600</v>
       </c>
       <c r="F9" s="9" t="s">
@@ -1070,12 +1194,299 @@
       </c>
       <c r="K11" s="9" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="204">
+      <c r="A12" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="7">
+        <v>43409</v>
+      </c>
+      <c r="D12" s="7">
+        <v>43409</v>
+      </c>
+      <c r="E12" s="11">
+        <f t="shared" si="2"/>
+        <v>1541376000</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="204">
+      <c r="A13" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="7">
+        <v>43411</v>
+      </c>
+      <c r="D13" s="7">
+        <v>43411</v>
+      </c>
+      <c r="E13" s="11">
+        <f t="shared" si="2"/>
+        <v>1541548800</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" t="s">
+        <v>74</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="187">
+      <c r="A14" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="7">
+        <v>43418</v>
+      </c>
+      <c r="D14" s="7">
+        <v>43418</v>
+      </c>
+      <c r="E14" s="11">
+        <f t="shared" si="2"/>
+        <v>1542153600</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" t="s">
+        <v>74</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="187">
+      <c r="A15" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="7">
+        <v>43423</v>
+      </c>
+      <c r="D15" s="7">
+        <v>43423</v>
+      </c>
+      <c r="E15" s="11">
+        <f t="shared" si="2"/>
+        <v>1542585600</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" t="s">
+        <v>74</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="153">
+      <c r="A16" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="7">
+        <v>43432</v>
+      </c>
+      <c r="D16" s="7">
+        <v>43432</v>
+      </c>
+      <c r="E16" s="11">
+        <f t="shared" si="2"/>
+        <v>1543363200</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" t="s">
+        <v>74</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="153">
+      <c r="A17" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="7">
+        <v>43437</v>
+      </c>
+      <c r="D17" s="7">
+        <v>43437</v>
+      </c>
+      <c r="E17" s="11">
+        <f t="shared" si="2"/>
+        <v>1543795200</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" t="s">
+        <v>74</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="238">
+      <c r="A18" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="7">
+        <v>43411</v>
+      </c>
+      <c r="D18" s="7">
+        <v>43411</v>
+      </c>
+      <c r="E18" s="11">
+        <f t="shared" si="2"/>
+        <v>1541548800</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="H18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" t="s">
+        <v>74</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="170">
+      <c r="A19" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="7">
+        <v>43412</v>
+      </c>
+      <c r="D19" s="7">
+        <v>43412</v>
+      </c>
+      <c r="E19" s="11">
+        <f t="shared" si="2"/>
+        <v>1541635200</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" xr:uid="{9FDCD70E-73D6-6E4B-93C8-7F50D40C1733}"/>
     <hyperlink ref="G9" r:id="rId2" xr:uid="{094A97C3-0E37-CD4B-BB28-AA16C6BF4C21}"/>
+    <hyperlink ref="G12" r:id="rId3" xr:uid="{BDB1237D-6C04-0A4C-98F9-40C57BDB08BA}"/>
+    <hyperlink ref="G18" r:id="rId4" xr:uid="{AAF51A9F-27C8-9742-9786-03247B3A5FF1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Updated with latest BCBB seminars
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E78F5C6-B4EA-C94C-A042-D2D0648E5694}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FA210B-41E8-AC44-A804-B7D4BDF51826}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17600" yWindow="460" windowWidth="33600" windowHeight="25380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="102">
   <si>
     <t>type</t>
   </si>
@@ -365,6 +365,22 @@
 Prof. Kiessling's talk is entitled "Probes of Dendritic Cell Lectins".
 The seminar will begin at 10:00 a.m. on Thursday, November 8, 2018, at NCI-Frederick in Bldg. 376, Room 121 on the Fort Detrick campus, Frederick, MD.   It will also be video-conferenced 'live' to Building 3, Room 2E04 on the Bethesda campus and Room E-1201 at the Advanced Technology Research Facility (ATRF).
 You will find Prof. Kiessling's bibliography at: https://ncifrederick.cancer.gov/ScientificLibrary/Bibliography/Default.aspx</t>
+  </si>
+  <si>
+    <t>How to Get the Most Out of Your Nephele Results</t>
+  </si>
+  <si>
+    <t>https://register.gotowebinar.com/register/3616787819082950657</t>
+  </si>
+  <si>
+    <t>Have you wondered how you might be able to better understand the Nephele pipeline results and get the most out of them? This webinar will cover best practices and tips on using the Nephele pipelines. 
+By attending this webinar, you will learn about the new Nephele pipelines and will get answers for: 
+• How do I check my data’s quality?
+• How do I explore my output files and troubleshoot problems?
+• How do I visualize my output further?</t>
+  </si>
+  <si>
+    <t>microbiome</t>
   </si>
 </sst>
 </file>
@@ -783,11 +799,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1105,7 +1121,7 @@
         <v>43398</v>
       </c>
       <c r="E9" s="11">
-        <f t="shared" ref="E9:E19" si="2">(C9-DATE(1970,1,1))*86400</f>
+        <f t="shared" ref="E9:E20" si="2">(C9-DATE(1970,1,1))*86400</f>
         <v>1540425600</v>
       </c>
       <c r="F9" s="9" t="s">
@@ -1479,6 +1495,42 @@
       </c>
       <c r="K19" s="9" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="119">
+      <c r="A20" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="7">
+        <v>43420</v>
+      </c>
+      <c r="D20" s="7">
+        <v>43420</v>
+      </c>
+      <c r="E20" s="11">
+        <f t="shared" si="2"/>
+        <v>1542326400</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" t="s">
+        <v>74</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with new events
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2600CD-DD2B-E049-A8A8-1A3306EAB4A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8948C71F-ACF4-8B40-8F48-6B750DF8BEA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17600" yWindow="460" windowWidth="33600" windowHeight="25380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
   <si>
     <t>type</t>
   </si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t>NIH Main Campus, Building 12, Room B51</t>
-  </si>
-  <si>
-    <t>Bioinformatics Programming with Python</t>
   </si>
   <si>
     <t>Building Workflows with Python</t>
@@ -177,17 +174,6 @@
   </si>
   <si>
     <t>python,Jupyter notebook</t>
-  </si>
-  <si>
-    <t>https://training.cit.nih.gov/class_details.aspx?cId=NIHCIT-SS460</t>
-  </si>
-  <si>
-    <t>In this seminar, we will explore the bioinformatics capabilities of the python programming language. We will examine some of the many capabilities of the biopython package as well as delve into the bioconda project for easy bioinformatics software installation. Students will receive a Jupyter Notebook with all steps taught in the class for further study and practice. 
-This seminar will be concurrently webcast for those who cannot attend in person (Register here: http://bit.ly/nih-python-register) 
-Prerequisites
-- Introduction to the Command Line webinar (http://bioinformatics.niaid.nih.gov)
-- Introduction to Jupiter notebook
-- Introduction to Programming (with Python) or previous programming experience required</t>
   </si>
   <si>
     <t>https://training.cit.nih.gov/class_details.aspx?cId=NIHCIT-SS470</t>
@@ -214,25 +200,6 @@
     <t>https://training.cit.nih.gov/class_details.aspx?cId=NIHCIT-SS497</t>
   </si>
   <si>
-    <t>https://register.gotowebinar.com/register/2903823797545605121</t>
-  </si>
-  <si>
-    <t>**This event is for NIH Staff only**
-METAGENOTE refers to the collection of metadata from genomics studies using a web-based notebook. METAGENOTE facilitates the annotation of datasets to ensure that metadata is stored in one centralized location for each group and automates the submission of files to the SRA. This tool, developed by NIAID, is freely accessible to all NIH researchers. 
-The webinar will cover easy ways to annotate your samples and submit them to the NCBI Sequence Read Archive (SRA) using METAGENOTE. 
-By attending this webinar, you can expect to learn:
-• What is METAGENOTE and why do I want to use it? 
-• How do I import metadata from Excel files? 
-• How do I share annotated sample group tables with lab members? 
-• How do I submit my sample data to the SRA database automatically?</t>
-  </si>
-  <si>
-    <t>genomic data,SRA</t>
-  </si>
-  <si>
-    <t>Introduction to METAGENOTE</t>
-  </si>
-  <si>
     <t>GoToWebinar</t>
   </si>
   <si>
@@ -262,6 +229,23 @@
   </si>
   <si>
     <t>microbiome</t>
+  </si>
+  <si>
+    <t>Walk-In Consult with HPC staff</t>
+  </si>
+  <si>
+    <t>Bldg 50 coffee shop area</t>
+  </si>
+  <si>
+    <t>Consult</t>
+  </si>
+  <si>
+    <t>All Helix or Biowulf users, and all those interested in using the systems, are invited to stop by and discuss problems and concerns, from scripting problems to node allocation, to strategies for a particular project, to anything that is affecting your use of Helix or Biowulf. We'll try to address simpler issues on the spot and follow up on more complex questions after the Walk-In.
+No appointments are necessary, and all problems are welcome.
+Look for the signs saying 'NIH HPC Walk-In Consults' on the tables to find us!</t>
+  </si>
+  <si>
+    <t>HPC</t>
   </si>
 </sst>
 </file>
@@ -271,7 +255,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -283,14 +267,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -348,11 +324,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -380,16 +355,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -668,7 +639,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -770,7 +741,7 @@
       <c r="B3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="16">
         <v>43438</v>
       </c>
       <c r="D3" s="12">
@@ -814,7 +785,7 @@
         <v>43642</v>
       </c>
       <c r="E4" s="10">
-        <f t="shared" ref="E4:E12" si="1">(C4-DATE(1970,1,1))*86400</f>
+        <f t="shared" ref="E4:E11" si="1">(C4-DATE(1970,1,1))*86400</f>
         <v>1561420800</v>
       </c>
       <c r="F4" s="9" t="s">
@@ -833,7 +804,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="204" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="187" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>34</v>
       </c>
@@ -841,32 +812,32 @@
         <v>36</v>
       </c>
       <c r="C5" s="7">
-        <v>43411</v>
+        <v>43418</v>
       </c>
       <c r="D5" s="7">
-        <v>43411</v>
+        <v>43418</v>
       </c>
       <c r="E5" s="10">
         <f t="shared" si="1"/>
-        <v>1541548800</v>
+        <v>1542153600</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>35</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H5" t="s">
         <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="187" x14ac:dyDescent="0.2">
@@ -877,35 +848,35 @@
         <v>37</v>
       </c>
       <c r="C6" s="7">
-        <v>43418</v>
+        <v>43423</v>
       </c>
       <c r="D6" s="7">
-        <v>43418</v>
+        <v>43423</v>
       </c>
       <c r="E6" s="10">
         <f t="shared" si="1"/>
-        <v>1542153600</v>
+        <v>1542585600</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>35</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H6" t="s">
         <v>14</v>
       </c>
       <c r="I6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="153" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>34</v>
       </c>
@@ -913,32 +884,32 @@
         <v>38</v>
       </c>
       <c r="C7" s="7">
-        <v>43423</v>
+        <v>43432</v>
       </c>
       <c r="D7" s="7">
-        <v>43423</v>
+        <v>43432</v>
       </c>
       <c r="E7" s="10">
         <f t="shared" si="1"/>
-        <v>1542585600</v>
+        <v>1543363200</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="H7" t="s">
         <v>14</v>
       </c>
       <c r="I7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="K7" s="9" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="153" x14ac:dyDescent="0.2">
@@ -949,14 +920,14 @@
         <v>39</v>
       </c>
       <c r="C8" s="7">
-        <v>43432</v>
+        <v>43437</v>
       </c>
       <c r="D8" s="7">
-        <v>43432</v>
+        <v>43437</v>
       </c>
       <c r="E8" s="10">
         <f t="shared" si="1"/>
-        <v>1543363200</v>
+        <v>1543795200</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>35</v>
@@ -968,160 +939,118 @@
         <v>14</v>
       </c>
       <c r="I8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>42</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="170" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C9" s="7">
-        <v>43437</v>
+        <v>43412</v>
       </c>
       <c r="D9" s="7">
-        <v>43437</v>
+        <v>43412</v>
       </c>
       <c r="E9" s="10">
         <f t="shared" si="1"/>
-        <v>1543795200</v>
+        <v>1541635200</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="H9" t="s">
         <v>14</v>
       </c>
       <c r="I9" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C10" s="7">
-        <v>43411</v>
+        <v>43420</v>
       </c>
       <c r="D10" s="7">
-        <v>43411</v>
+        <v>43420</v>
       </c>
       <c r="E10" s="10">
         <f t="shared" si="1"/>
-        <v>1541548800</v>
+        <v>1542326400</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="H10" t="s">
         <v>14</v>
       </c>
       <c r="I10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="136" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>60</v>
       </c>
       <c r="C11" s="7">
-        <v>43412</v>
+        <v>43418</v>
       </c>
       <c r="D11" s="7">
-        <v>43412</v>
+        <v>43418</v>
       </c>
       <c r="E11" s="10">
         <f t="shared" si="1"/>
-        <v>1541635200</v>
+        <v>1542153600</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>61</v>
       </c>
       <c r="H11" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="I11" t="s">
         <v>13</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="119" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="7">
-        <v>43420</v>
-      </c>
-      <c r="D12" s="7">
-        <v>43420</v>
-      </c>
-      <c r="E12" s="10">
-        <f t="shared" si="1"/>
-        <v>1542326400</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="H12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G10" r:id="rId1" xr:uid="{AAF51A9F-27C8-9742-9786-03247B3A5FF1}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated with new events 11/21
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dolanmi/Desktop/bcbb/products/nbp/events/nbp_events_niaid/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E38E283-20E8-F041-AECD-897E7218EE60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC40496-22ED-4041-909F-31009BC976FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="4380" windowWidth="28260" windowHeight="12520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22740" yWindow="460" windowWidth="27580" windowHeight="21340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>type</t>
   </si>
@@ -102,9 +102,6 @@
     <t>immunology</t>
   </si>
   <si>
-    <t>STRUCTBIOLIG listserv</t>
-  </si>
-  <si>
     <t>https://clue.io/workshop2018</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>Broad Institute, 415 Main St., Cambridge, MA 02142</t>
   </si>
   <si>
-    <t>molecular discovery</t>
-  </si>
-  <si>
     <t>Rockefeller University</t>
   </si>
   <si>
@@ -136,12 +130,6 @@
   </si>
   <si>
     <t>NIH Main Campus, Building 12, Room B51</t>
-  </si>
-  <si>
-    <t>Building Workflows with Python</t>
-  </si>
-  <si>
-    <t>Biomedical Data Storage and Retrieval (using SQL &amp; NoSQL)</t>
   </si>
   <si>
     <t>Becoming a Reproducible Scientist (Part 1)</t>
@@ -170,85 +158,40 @@
     <t>https://training.cit.nih.gov/class_details.aspx?cId=NIHCIT-SS500</t>
   </si>
   <si>
-    <t>python,Jupyter notebook</t>
-  </si>
-  <si>
-    <t>https://training.cit.nih.gov/class_details.aspx?cId=NIHCIT-SS470</t>
-  </si>
-  <si>
-    <t>In this seminar, we will assemble a working pipeline based upon the steps we have learned in the previous seminars while surveying a few methods for building workflows, including the snakemake package. Students will receive a Jupyter Notebook with all steps taught in the class for further study and practice. 
-This seminar will be concurrently webcast for those who cannot attend in person (Register here: http://bit.ly/nih-python-register) 
-Prerequisites
-- Introduction to the Command Line webinar (http://bioinformatics.niaid.nih.gov)
-- Introduction to Jupiter notebook
-- Introduction to Programming (with Python) or previous programming experience required</t>
-  </si>
-  <si>
-    <t>Biological data continues to grow at an incredible rate! In the seminar, we will examine data storage and retrieval strategies, use cases, and practical examples using databases (including MySQL and MongoDB) as well as programming languages to access them (SQL and NoSQL). Programming will be done using the Python programming language. Students will receive a Jupyter Notebook with all steps taught in the class for further study and practice. 
-This seminar will be concurrently webcast for those who cannot attend in person (Register here: http://bit.ly/nih-python-register) 
-Prerequisites
-- Experience with a computer and web browser
-- Familiarity with the Python programming language</t>
-  </si>
-  <si>
-    <t>data storage, MySQL,MongoDB,Jupyter notebook</t>
-  </si>
-  <si>
-    <t>https://training.cit.nih.gov/class_details.aspx?cId=NIHCIT-SS497</t>
-  </si>
-  <si>
-    <t>GoToWebinar</t>
-  </si>
-  <si>
-    <t>Probes of Dendritic Cell Lectins</t>
-  </si>
-  <si>
-    <t>NCI-Frederick Fort Detrick campus, Bldg. 376, Room 121</t>
-  </si>
-  <si>
-    <t>NCI at Frederick is pleased to announce a forthcoming seminar in the "Molecular Discovery Seminar Series (MDSS)."  The presenter will be Prof. Laura L. Kiessling*, Massachusetts Institute of Technology (MIT), Dept. of Chemistry, Cambridge, MA.
-Prof. Kiessling's talk is entitled "Probes of Dendritic Cell Lectins".
-The seminar will begin at 10:00 a.m. on Thursday, November 8, 2018, at NCI-Frederick in Bldg. 376, Room 121 on the Fort Detrick campus, Frederick, MD.   It will also be video-conferenced 'live' to Building 3, Room 2E04 on the Bethesda campus and Room E-1201 at the Advanced Technology Research Facility (ATRF).
-You will find Prof. Kiessling's bibliography at: https://ncifrederick.cancer.gov/ScientificLibrary/Bibliography/Default.aspx</t>
-  </si>
-  <si>
-    <t>How to Get the Most Out of Your Nephele Results</t>
-  </si>
-  <si>
-    <t>https://register.gotowebinar.com/register/3616787819082950657</t>
-  </si>
-  <si>
-    <t>Have you wondered how you might be able to better understand the Nephele pipeline results and get the most out of them? This webinar will cover best practices and tips on using the Nephele pipelines. 
-By attending this webinar, you will learn about the new Nephele pipelines and will get answers for: 
-• How do I check my data’s quality?
-• How do I explore my output files and troubleshoot problems?
-• How do I visualize my output further?</t>
-  </si>
-  <si>
     <t>microbiome</t>
   </si>
   <si>
-    <t>Walk-In Consult with HPC staff</t>
-  </si>
-  <si>
-    <t>Bldg 50 coffee shop area</t>
-  </si>
-  <si>
-    <t>Consult</t>
-  </si>
-  <si>
-    <t>All Helix or Biowulf users, and all those interested in using the systems, are invited to stop by and discuss problems and concerns, from scripting problems to node allocation, to strategies for a particular project, to anything that is affecting your use of Helix or Biowulf. We'll try to address simpler issues on the spot and follow up on more complex questions after the Walk-In.
-No appointments are necessary, and all problems are welcome.
-Look for the signs saying 'NIH HPC Walk-In Consults' on the tables to find us!</t>
-  </si>
-  <si>
-    <t>HPC</t>
-  </si>
-  <si>
     <t>http://bioc2018.bioconductor.org</t>
   </si>
   <si>
     <t xml:space="preserve"> To see a list of past workshops, visit http://bioc2018.bioconductor.org.</t>
+  </si>
+  <si>
+    <t>MICROBIOME listserv</t>
+  </si>
+  <si>
+    <t>The bugs within and around us: understanding complex microbial communities with next-generation sequencing</t>
+  </si>
+  <si>
+    <t>Hilton Washington DC/Rockville Hotel &amp; Executive Meeting Ctr, 1750 Rockville Pike, Room: Potomac Room, Rockville, Maryland</t>
+  </si>
+  <si>
+    <t>https://www.illumina.com/events/seminars.html</t>
+  </si>
+  <si>
+    <t>Come join us in a social event to discuss various ways NGS has been used to characterize bacterial and viral pathogens. We will explore the different scientific approaches and gain insight into how to improve human health through topics on microbial communities in veal calves and dairy animals and to Ebola outbreak management in the Democratic Republic of the Congo.</t>
+  </si>
+  <si>
+    <t>The course will begin with the workflow involved in moving from platform images to sequence generation, after which participants will gain practical skills for evaluating sequence read quality, mapping reads to a reference genome, and analyzing sequence reads for variation and expression level. The course will conclude with pathway and network analysis on the resultant 'gene' list. Participants will gain experience in cloud computing and data visualization tools. All class exercises will be self-contained units that include example data (e.g., Illumina paired-end data) as well as detailed instructions for installing all required bioinformatics tools.</t>
+  </si>
+  <si>
+    <t>High-Throughput Biology: From Sequence to Networks CSHL Course</t>
+  </si>
+  <si>
+    <t>https://meetings.cshl.edu/courses.aspx?course=C-cbw&amp;year=19</t>
+  </si>
+  <si>
+    <t>1 Bungtown Road Cold Spring Harbor, NY 11724-2213</t>
   </si>
 </sst>
 </file>
@@ -655,11 +598,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -755,7 +698,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="16">
         <v>43438</v>
@@ -768,10 +711,10 @@
         <v>1543881600</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>21</v>
@@ -780,10 +723,10 @@
         <v>13</v>
       </c>
       <c r="J3" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="L3" s="14"/>
     </row>
@@ -792,7 +735,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" s="7">
         <v>43641</v>
@@ -801,14 +744,14 @@
         <v>43642</v>
       </c>
       <c r="E4" s="10">
-        <f t="shared" ref="E4:E11" si="1">(C4-DATE(1970,1,1))*86400</f>
+        <f t="shared" ref="E4:E8" si="1">(C4-DATE(1970,1,1))*86400</f>
         <v>1561420800</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>21</v>
@@ -817,261 +760,157 @@
         <v>13</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="153" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>35</v>
-      </c>
       <c r="C5" s="7">
-        <v>43418</v>
+        <v>43432</v>
       </c>
       <c r="D5" s="7">
-        <v>43418</v>
+        <v>43432</v>
       </c>
       <c r="E5" s="10">
         <f t="shared" si="1"/>
-        <v>1542153600</v>
+        <v>1543363200</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="H5" t="s">
         <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="153" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" s="7">
-        <v>43423</v>
+        <v>43437</v>
       </c>
       <c r="D6" s="7">
-        <v>43423</v>
+        <v>43437</v>
       </c>
       <c r="E6" s="10">
         <f t="shared" si="1"/>
-        <v>1542585600</v>
+        <v>1543795200</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H6" t="s">
         <v>14</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C7" s="7">
-        <v>43432</v>
+        <v>43440</v>
       </c>
       <c r="D7" s="7">
-        <v>43432</v>
+        <v>43440</v>
       </c>
       <c r="E7" s="10">
         <f t="shared" si="1"/>
-        <v>1543363200</v>
+        <v>1544054400</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H7" t="s">
         <v>14</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C8" s="7">
-        <v>43437</v>
+        <v>43535</v>
       </c>
       <c r="D8" s="7">
-        <v>43437</v>
+        <v>43541</v>
       </c>
       <c r="E8" s="10">
         <f t="shared" si="1"/>
-        <v>1543795200</v>
+        <v>1552262400</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>44</v>
+        <v>52</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>51</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="170" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="7">
-        <v>43412</v>
-      </c>
-      <c r="D9" s="7">
-        <v>43412</v>
-      </c>
-      <c r="E9" s="10">
-        <f t="shared" si="1"/>
-        <v>1541635200</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="119" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="7">
-        <v>43420</v>
-      </c>
-      <c r="D10" s="7">
-        <v>43420</v>
-      </c>
-      <c r="E10" s="10">
-        <f t="shared" si="1"/>
-        <v>1542326400</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="136" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="7">
-        <v>43418</v>
-      </c>
-      <c r="D11" s="7">
-        <v>43418</v>
-      </c>
-      <c r="E11" s="10">
-        <f t="shared" si="1"/>
-        <v>1542153600</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" t="s">
-        <v>61</v>
-      </c>
-      <c r="I11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" xr:uid="{1E644AB0-1CE4-CA43-BC4B-C485696BC585}"/>
+    <hyperlink ref="G8" r:id="rId2" xr:uid="{435D4641-689C-4342-BC3A-BE8C2BA92CAC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Updated files with new events
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3739C7B2-790B-DF43-B702-F4490D492642}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C874FB-49BB-A547-94F6-393DC37F4FE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26040" yWindow="460" windowWidth="27580" windowHeight="21340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23620" yWindow="460" windowWidth="27580" windowHeight="21340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>type</t>
   </si>
@@ -102,21 +102,6 @@
     <t>immunology</t>
   </si>
   <si>
-    <t>https://clue.io/workshop2018</t>
-  </si>
-  <si>
-    <t>Connectivity Map Workshop</t>
-  </si>
-  <si>
-    <t>A suite of training modules aimed at users of L1000 and LINCS data will be offered. Content will be geared toward people familiar with Connectivity Map or gene expression analysis.</t>
-  </si>
-  <si>
-    <t>connectivitymap, gene expression</t>
-  </si>
-  <si>
-    <t>Broad Institute, 415 Main St., Cambridge, MA 02142</t>
-  </si>
-  <si>
     <t>Rockefeller University</t>
   </si>
   <si>
@@ -126,28 +111,9 @@
     <t>bioconductor,genomic data</t>
   </si>
   <si>
-    <t>NIH Calendar of Events</t>
-  </si>
-  <si>
-    <t>NIH Main Campus, Building 12, Room B51</t>
-  </si>
-  <si>
-    <t>Becoming a Reproducible Scientist (Part 2)</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
-    <t xml:space="preserve">We will explore reasons for reproducible science and delve into practical exercises that will allow you to enhance your data analysis with good, better, and best practices. Topics include introduction to Jupyter Notebook, basic intro to the python programming language, data and project organization, data exploration, automation, publishing, and sharing. This seminar will condense the Data Carpentry Reproducible Science Jupyter workshop held in Berkeley, CA in 2017 &amp; 2018 (https://github.com/Reproducible-Science-Curriculum). Students will receive a Jupyter Notebook with all steps taught in the class for further study and practice. 
-This seminar will be concurrently webcast for those who cannot attend in person (Register here: http://bit.ly/nih-python-register) </t>
-  </si>
-  <si>
-    <t>reproducibility</t>
-  </si>
-  <si>
-    <t>https://training.cit.nih.gov/class_details.aspx?cId=NIHCIT-SS500</t>
-  </si>
-  <si>
     <t>microbiome</t>
   </si>
   <si>
@@ -196,9 +162,6 @@
     <t>Electronic Lab Notebook (ELN) Discussion</t>
   </si>
   <si>
-    <t>https://www.nihlibrary.nih.gov/training/invitation-participate-electronic-lab-notebook-online-discussion-session-3</t>
-  </si>
-  <si>
     <t>Discussion</t>
   </si>
   <si>
@@ -206,24 +169,6 @@
   </si>
   <si>
     <t>https://www.nihlibrary.nih.gov/training/invitation-participate-electronic-lab-notebook-online-discussion-session-4</t>
-  </si>
-  <si>
-    <t>STRUCTBIOLIG listserv</t>
-  </si>
-  <si>
-    <t>Structure and Signaling Mechanisms of G Protein-Coupled and b-Arrestin-Biased Chemokine Receptors</t>
-  </si>
-  <si>
-    <t>NIH Main Campus, Building 10, Lipsett Auditorium</t>
-  </si>
-  <si>
-    <t>Most chemokine receptors are G Protein-Coupled Receptors (GPCRs), and are best known for their role in controlling cell migration in the context of immune system function. They are also implicated in many diseases particularly inflammatory diseases as well as cancer and HIV, making them important therapeutic targets. Recent structural and biophysical studies have revealed that the recognition interface between chemokines and receptors is very large and characterized by more complex epitopes than previously believed.  In this presentation, our current understanding of how chemokines bind and activate their receptors will be described, as well mechanisms for inhibiting chemokine receptor signaling with orthosteric and allosteric ligands.  Common and unique features of G protein-coupled versus b-arrestin-biased receptors will also be described, focusing on CXCR4 (a GPCR) and the b -arrestin-biased, atypical chemokine receptor 3 (ACKR3) both of which respond to the chemokine CXCL12.</t>
-  </si>
-  <si>
-    <t>chemokine</t>
-  </si>
-  <si>
-    <t>Lecture</t>
   </si>
   <si>
     <t>https://www.surveymonkey.com/r/Feb2019_NCBI_hackathon</t>
@@ -241,6 +186,29 @@
   </si>
   <si>
     <t>NCBI Biodata Science Hackathon</t>
+  </si>
+  <si>
+    <t>Walk-In Consult with HPC staff</t>
+  </si>
+  <si>
+    <t>NIH Main Campus, Bldg 35A (Porter Neuroscience Building) lobby</t>
+  </si>
+  <si>
+    <t>Consultation</t>
+  </si>
+  <si>
+    <t>All Helix or Biowulf users, and all those interested in using the systems,
+are invited to stop by and discuss problems and concerns, from scripting
+problems to node allocation, to strategies for a particular project, to
+anything that is affecting your use of Helix or Biowulf. We'll try to
+address simpler issues on the spot and follow up on more complex
+questions after the Walk-In.
+No appointments are necessary, and all problems are welcome.
+Look for the signs saying 'NIH HPC Walk-In Consults' on the tables to
+find us!</t>
+  </si>
+  <si>
+    <t>HPC,Helix,Biowulf</t>
   </si>
 </sst>
 </file>
@@ -250,7 +218,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -262,20 +230,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF0A0101"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -329,9 +283,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -359,14 +313,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -648,11 +598,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -743,28 +693,28 @@
       </c>
       <c r="L2" s="14"/>
     </row>
-    <row r="3" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="16">
-        <v>43438</v>
-      </c>
-      <c r="D3" s="12">
-        <v>43440</v>
+      <c r="C3" s="7">
+        <v>43641</v>
+      </c>
+      <c r="D3" s="7">
+        <v>43642</v>
       </c>
       <c r="E3" s="10">
-        <f t="shared" ref="E3" si="0">(C3-DATE(1970,1,1))*86400</f>
-        <v>1543881600</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="11" t="s">
+        <f t="shared" ref="E3:E8" si="0">(C3-DATE(1970,1,1))*86400</f>
+        <v>1561420800</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>23</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>28</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>21</v>
@@ -772,298 +722,189 @@
       <c r="I3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="14"/>
     </row>
-    <row r="4" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="7">
+        <v>43440</v>
+      </c>
+      <c r="D4" s="7">
+        <v>43440</v>
+      </c>
+      <c r="E4" s="10">
+        <f t="shared" si="0"/>
+        <v>1544054400</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="7">
-        <v>43641</v>
-      </c>
-      <c r="D4" s="7">
-        <v>43642</v>
-      </c>
-      <c r="E4" s="10">
-        <f t="shared" ref="E4:E11" si="1">(C4-DATE(1970,1,1))*86400</f>
-        <v>1561420800</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="10" t="s">
+      <c r="B5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="7">
+        <v>43535</v>
+      </c>
+      <c r="D5" s="7">
+        <v>43541</v>
+      </c>
+      <c r="E5" s="10">
+        <f t="shared" si="0"/>
+        <v>1552262400</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I5" t="s">
         <v>13</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="153" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="7">
-        <v>43437</v>
-      </c>
-      <c r="D5" s="7">
-        <v>43437</v>
-      </c>
-      <c r="E5" s="10">
-        <f t="shared" si="1"/>
-        <v>1543795200</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" t="s">
-        <v>34</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>42</v>
       </c>
       <c r="C6" s="7">
-        <v>43440</v>
+        <v>43473</v>
       </c>
       <c r="D6" s="7">
-        <v>43440</v>
+        <v>43473</v>
       </c>
       <c r="E6" s="10">
-        <f t="shared" si="1"/>
-        <v>1544054400</v>
+        <f t="shared" si="0"/>
+        <v>1546905600</v>
       </c>
       <c r="F6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
       <c r="I6" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="187" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C7" s="7">
-        <v>43535</v>
+        <v>43516</v>
       </c>
       <c r="D7" s="7">
-        <v>43541</v>
+        <v>43518</v>
       </c>
       <c r="E7" s="10">
-        <f t="shared" si="1"/>
-        <v>1552262400</v>
-      </c>
-      <c r="F7" s="9" t="s">
+        <f t="shared" si="0"/>
+        <v>1550620800</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" t="s">
         <v>49</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" t="s">
-        <v>21</v>
       </c>
       <c r="I7" t="s">
         <v>13</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="187" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="7">
+        <v>43446</v>
+      </c>
+      <c r="D8" s="7">
+        <v>43446</v>
+      </c>
+      <c r="E8" s="10">
+        <f t="shared" si="0"/>
+        <v>1544572800</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="7">
-        <v>43439</v>
-      </c>
-      <c r="D8" s="7">
-        <v>43439</v>
-      </c>
-      <c r="E8" s="10">
-        <f t="shared" si="1"/>
-        <v>1543968000</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="9" t="s">
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H8" t="s">
+      <c r="K8" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="I8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="68" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="7">
-        <v>43473</v>
-      </c>
-      <c r="D9" s="7">
-        <v>43473</v>
-      </c>
-      <c r="E9" s="10">
-        <f t="shared" si="1"/>
-        <v>1546905600</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" t="s">
-        <v>55</v>
-      </c>
-      <c r="I9" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="153" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="7">
-        <v>43439</v>
-      </c>
-      <c r="D10" s="7">
-        <v>43439</v>
-      </c>
-      <c r="E10" s="10">
-        <f t="shared" si="1"/>
-        <v>1543968000</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="H10" t="s">
-        <v>63</v>
-      </c>
-      <c r="I10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="187" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="7">
-        <v>43516</v>
-      </c>
-      <c r="D11" s="7">
-        <v>43518</v>
-      </c>
-      <c r="E11" s="10">
-        <f t="shared" si="1"/>
-        <v>1550620800</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G4" r:id="rId1" xr:uid="{1E644AB0-1CE4-CA43-BC4B-C485696BC585}"/>
-    <hyperlink ref="G7" r:id="rId2" xr:uid="{435D4641-689C-4342-BC3A-BE8C2BA92CAC}"/>
-    <hyperlink ref="G11" r:id="rId3" xr:uid="{42D7B41B-1B43-9345-AA3D-5EB4146C3F1E}"/>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{1E644AB0-1CE4-CA43-BC4B-C485696BC585}"/>
+    <hyperlink ref="G5" r:id="rId2" xr:uid="{435D4641-689C-4342-BC3A-BE8C2BA92CAC}"/>
+    <hyperlink ref="G7" r:id="rId3" xr:uid="{42D7B41B-1B43-9345-AA3D-5EB4146C3F1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Removed old events from 2018
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC43A694-C080-0943-A8B7-71D9E06A05AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85812222-EEFE-7943-B8BF-9B897C9CDE03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28920" yWindow="460" windowWidth="27580" windowHeight="21340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6020" yWindow="460" windowWidth="27580" windowHeight="19740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>type</t>
   </si>
@@ -75,9 +75,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>Seminar</t>
-  </si>
-  <si>
     <t>BIOINFO-GENERAL-NCI listserv</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
   </si>
   <si>
     <t xml:space="preserve"> To see a list of past workshops, visit http://bioc2018.bioconductor.org.</t>
-  </si>
-  <si>
-    <t>MICROBIOME listserv</t>
   </si>
   <si>
     <t>The course will begin with the workflow involved in moving from platform images to sequence generation, after which participants will gain practical skills for evaluating sequence read quality, mapping reads to a reference genome, and analyzing sequence reads for variation and expression level. The course will conclude with pathway and network analysis on the resultant 'gene' list. Participants will gain experience in cloud computing and data visualization tools. All class exercises will be self-contained units that include example data (e.g., Illumina paired-end data) as well as detailed instructions for installing all required bioinformatics tools.</t>
@@ -171,33 +165,6 @@
   </si>
   <si>
     <t>NCBI Biodata Science Hackathon</t>
-  </si>
-  <si>
-    <t>Mechanisms involved in the prevention of type 1 diabetes onset by Lactobacillus johnsonii N6.2</t>
-  </si>
-  <si>
-    <t>Webinar</t>
-  </si>
-  <si>
-    <t>A myriad of complex host-microbe interactions occur in the gastrointestinal tract, some of which have been found to alter the development of type 1 diabetes (T1D) in animal models. Several microbiome studies have corroborated these findings in subjects with T1D. In Biobreeding diabetes-prone (BBDP) rats, it was  found a strong negative correlation between administration of the probiotic Lactobacillus johnsonii N6.2 and the development of autoimmunity (T1D). Mechanistically, it was determined that L. johnsonii N6.2 alters the host kynurenine pathway through modulation of the indoleamine 2,3-dioxygenase (IDO) enzyme. Metabolomics and immunophenotyping assays indicated shifts in the metabolites of the kynurenine pathway, as well as significant shifts in several immune cell frequencies in human subjects. In rodent models of disease, it was recently found that L. johnsonii N6.2 is able to dampen caspase 1-mediated inflammasome activation as well as reduce mTOR activating phosphorylations. Dr. Lorca's lab is currently focused on the identification of the bacterial effector molecules responsible for the effects observed using a variety of omics techniques.</t>
-  </si>
-  <si>
-    <t>https://cbiit.webex.com/cbiit/j.php?MTID=me7fa4356a7aafc80a26cf708855040dd</t>
-  </si>
-  <si>
-    <t>NCI Containers and Workflows Interest Group Seminar</t>
-  </si>
-  <si>
-    <t>https://cbiit.webex.com/cbiit/j.php?MTID=ma3f0d94985bbd365d114c5a469359aca</t>
-  </si>
-  <si>
-    <t>Jupyter Notebooks are interactive computing environments that allow users to implement and share computational results and methodologies, using a variety of formats and scripting languages, thus streamlining research processes which require in-depth analysis of large quantities of data. By launching an interactive analysis environment with a Jupyter Notebook on Firecloud - the Broad Institute’s open-source platform for accessing data, code, and processing resources - users can explore the workflows of their peers, share workspaces with their collaborators, and even reproduce published results. This webinar focuses on reproduction of results in a recent study (https://www.biorxiv.org/content/early/2018/04/13/300905) on the correlation between certain genetic variants and a common congenital heart condition. This exercise will serve as an instructive example for accessing data and methodologies shared on FireCloud, and running a notebook in order to manipulate and extract data.</t>
-  </si>
-  <si>
-    <t>microbiome,gastrointestinal</t>
-  </si>
-  <si>
-    <t>Jupyter</t>
   </si>
   <si>
     <t xml:space="preserve">Come join us for our next Bioinformatics User Forum meeting on Jan 11 in the ATRF Auditorium in Frederick. Our main speaker, Vishal Koparde, will be presenting a use-case on developing an NGS analysis pipeline in the cloud, and then we will break into small groups for roundtable discussions. </t>
@@ -602,11 +569,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -665,7 +632,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="12">
         <v>43537</v>
@@ -678,31 +645,31 @@
         <v>1552435200</v>
       </c>
       <c r="F2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>20</v>
-      </c>
       <c r="H2" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L2" s="14"/>
     </row>
     <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="7">
         <v>43641</v>
@@ -711,34 +678,34 @@
         <v>43642</v>
       </c>
       <c r="E3" s="10">
-        <f t="shared" ref="E3:E9" si="0">(C3-DATE(1970,1,1))*86400</f>
+        <f t="shared" ref="E3:E7" si="0">(C3-DATE(1970,1,1))*86400</f>
         <v>1561420800</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3" s="10" t="s">
         <v>13</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" s="7">
         <v>43535</v>
@@ -751,27 +718,27 @@
         <v>1552262400</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" t="s">
         <v>13</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" s="7">
         <v>43473</v>
@@ -784,22 +751,22 @@
         <v>1546905600</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="187" x14ac:dyDescent="0.2">
@@ -807,7 +774,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C6" s="7">
         <v>43516</v>
@@ -820,124 +787,52 @@
         <v>1550620800</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I6" t="s">
         <v>13</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="7">
-        <v>43448</v>
+        <v>43476</v>
       </c>
       <c r="D7" s="7">
-        <v>43448</v>
+        <v>43476</v>
       </c>
       <c r="E7" s="10">
         <f t="shared" si="0"/>
-        <v>1544745600</v>
+        <v>1547164800</v>
       </c>
       <c r="F7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" t="s">
-        <v>14</v>
-      </c>
       <c r="I7" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="J7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="153" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="7">
-        <v>43448</v>
-      </c>
-      <c r="D8" s="7">
-        <v>43448</v>
-      </c>
-      <c r="E8" s="10">
-        <f t="shared" si="0"/>
-        <v>1544745600</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="7">
-        <v>43476</v>
-      </c>
-      <c r="D9" s="7">
-        <v>43476</v>
-      </c>
-      <c r="E9" s="10">
-        <f t="shared" si="0"/>
-        <v>1547164800</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -945,7 +840,6 @@
     <hyperlink ref="G3" r:id="rId1" xr:uid="{1E644AB0-1CE4-CA43-BC4B-C485696BC585}"/>
     <hyperlink ref="G4" r:id="rId2" xr:uid="{435D4641-689C-4342-BC3A-BE8C2BA92CAC}"/>
     <hyperlink ref="G6" r:id="rId3" xr:uid="{42D7B41B-1B43-9345-AA3D-5EB4146C3F1E}"/>
-    <hyperlink ref="G8" r:id="rId4" xr:uid="{78D5F4F6-D38B-234A-9048-E8E0FAF207E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Removed old events and updated with new postings
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393F0E1F-9E31-594E-A4BD-55D3DED80798}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542B3F3B-452F-AD42-AD54-0CB3FA12F44E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22720" yWindow="620" windowWidth="27580" windowHeight="19740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
   <si>
     <t>type</t>
   </si>
@@ -149,19 +149,7 @@
     <t>NCBI Biodata Science Hackathon</t>
   </si>
   <si>
-    <t xml:space="preserve">Come join us for our next Bioinformatics User Forum meeting on Jan 11 in the ATRF Auditorium in Frederick. Our main speaker, Vishal Koparde, will be presenting a use-case on developing an NGS analysis pipeline in the cloud, and then we will break into small groups for roundtable discussions. </t>
-  </si>
-  <si>
-    <t>Bioinformatics User Forum Meeting</t>
-  </si>
-  <si>
-    <t>ATRF Auditorium, Frederick, MD</t>
-  </si>
-  <si>
     <t>Meeting</t>
-  </si>
-  <si>
-    <t>NGS analysis,tumor variant analysis,PATRIC,image analysis</t>
   </si>
   <si>
     <t>Electronic Lab Notebook (ELN) Forum</t>
@@ -200,45 +188,6 @@
     <t>statistics,data analysis,R</t>
   </si>
   <si>
-    <t>Walk-In Consult with HPC staff</t>
-  </si>
-  <si>
-    <t>NIH Main Campus, Bldg 10 (Clinical Center) atrium coffee shop area</t>
-  </si>
-  <si>
-    <t>Consult</t>
-  </si>
-  <si>
-    <t>All Helix or Biowulf users, and all those interested in using the systems,
-are invited to stop by and discuss problems and concerns, from scripting
-problems to node allocation, to strategies for a particular project, to
-anything that is affecting your use of Helix or Biowulf. We'll try to
-address simpler issues on the spot and follow up on more complex
-questions after the Walk-In.
-No appointments are necessary, and all problems are welcome.
-Look for the signs saying 'NIH HPC Walk-In Consults' on the tables to
-find us!</t>
-  </si>
-  <si>
-    <t>HPC,Helix,Biowulf</t>
-  </si>
-  <si>
-    <t>https://wiki.nci.nih.gov/display/CBIITSpeakers/CBIIT+Speaker+Series+Page</t>
-  </si>
-  <si>
-    <t>BioThings API: Building a FAIR API Ecosystem for Biomedical Knowledge</t>
-  </si>
-  <si>
-    <t>NCI Shady Grove Campus, Rm. 1W032-34</t>
-  </si>
-  <si>
-    <t>Building a web-based API (Application Programming Interface) has been rapidly adopted in the bioinformatics field as a new way of disseminating the underlying biomedical knowledge. While researchers benefit from the simplicity and the high accessibility (A) of available APIs, the findability (F), interoperability (I) and reusability (R) across APIs are largely not well-handled by the community. BioThings API project (http://biothings.io) is tasked to build a FAIR API ecosystem to better serve the underlying inter-connected biomedical knowledge. BioThings API provides three components in its API development ecosystem. First, it provides a family of high-performance APIs for accessing up-to-date annotations for genes, genetic variants, chemicals and drugs. Second, BioThings API packages its API-development best practice into a reusable SDK (Software Development Kit) to help other bioinformaticians to build the same high-quality API to distribute their own specific knowledge. Third, BioThings API provides a platform to foster the findability and interoperability across the community-developed biomedical APIs. Through the SmartAPI application (http://smart-api.info), it provides tools for authoring API metadata following the community supported OpenAPI standard and hosts standardized interactive API documentation. It also defines a set of OpenAPI extensions to provide biomedical-specific semantic annotations, such as what specific biomedical identifiers an API parameter accepts and what specific biomedical entity types an API response contains. Powered by these semantic annotations, a new web application called BioThings Explorer was developed to allow researchers to navigate the scope of the distributed biomedical API landscape and build the desired knowledge extraction workflows by identifying and combining required APIs.
-Our speaker will be presenting remotely. Please join  us via WebEx and register now to attend the presentation https://cbiit.webex.com/mw3300/mywebex/default.do?nomenu=true&amp;siteurl=cbiit&amp;service=6&amp;rnd=0.36559810657011804&amp;main_url=https%3A%2F%2Fcbiit.webex.com%2Fec3300%2Feventcenter%2Fevent%2FeventAction.do%3FtheAction%3Ddetail%26%26%26EMK%3D4832534b00000004abc0c3bd8aea855fdfc06a8bf7ec604e46193398ac2101c01417383149f9a1b0%26siteurl%3Dcbiit%26confViewID%3D113414922722877987%26encryptTicket%3DSDJTSwAAAATyuN5LZ9RcgKZAR0ywScNZWO1xMAf-S5izZFdfifKotA2%26</t>
-  </si>
-  <si>
-    <t>API,FAIR,biomedical knowledge extraction</t>
-  </si>
-  <si>
     <t>NICBR Winter Symposium "Novel Therapeutics"</t>
   </si>
   <si>
@@ -264,6 +213,42 @@
   </si>
   <si>
     <t>NIH Main Campus</t>
+  </si>
+  <si>
+    <t>HFIR/SNS Advanced Neutron Diffraction and Scattering Workshop</t>
+  </si>
+  <si>
+    <t>STRUCTBIOLIG listserv</t>
+  </si>
+  <si>
+    <t>The workshop aims at enabling structural biologists to fully exploit the latest instrumentation and software development at the SNS and HFIR facilities at Oak Ridge National Laboratory. Participants of HANDS 2019 will become familiar with neutron techniques with hands-on experiments in sample preparation, crystallography, small angle scattering, reflectometry and neutron spin echo. The workshop is designed for graduate students, post-doctoral fellows and faculty with limited to no experience with neutron sciences.</t>
+  </si>
+  <si>
+    <t>structural biology,neutron techniques</t>
+  </si>
+  <si>
+    <t>https://conference.sns.gov/event/125/</t>
+  </si>
+  <si>
+    <t>Oak Ridge National Laboratory, 8640 Nano Center Drive Oak Ridge, TN 37830</t>
+  </si>
+  <si>
+    <t>Generating High-quality Genome Drafts from Uncultured Microbiome Samples with a Single Shotgun Experiment</t>
+  </si>
+  <si>
+    <t>https://www.10xgenomics.com/event/generating-high-quality-genome-drafts-from-uncultured-microbiome-samples/</t>
+  </si>
+  <si>
+    <t>Webinar</t>
+  </si>
+  <si>
+    <t>This webinar will feature a presentation on a recently published method for de novo assembly of microbial genome drafts using short read sequencing. The method uses Chromium Linked-Read sequencing and a novel computational analysis pipeline, Athena, to construct high-quality microbial genome drafts of metagenomic communities sampled directly from their environments. In uncultured samples from human stool, Athena produced individual genome drafts with high contiguity (&gt;200-kb N50, fewer than ten contigs), even for bacteria with relatively low raw short-read sequence coverage. Compared with results from existing short-read and synthetic long-read metagenomic sequencing techniques, the Athena assemblies are the most contiguous reported to date.</t>
+  </si>
+  <si>
+    <t>de novo assembly,Athena,short-read sequencing</t>
+  </si>
+  <si>
+    <t>Online only</t>
   </si>
 </sst>
 </file>
@@ -653,11 +638,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -762,7 +747,7 @@
         <v>43642</v>
       </c>
       <c r="E3" s="10">
-        <f t="shared" ref="E3:E11" si="0">(C3-DATE(1970,1,1))*86400</f>
+        <f t="shared" ref="E3:E10" si="0">(C3-DATE(1970,1,1))*86400</f>
         <v>1561420800</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -835,10 +820,10 @@
         <v>1550620800</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="H5" t="s">
         <v>36</v>
@@ -853,55 +838,58 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>39</v>
       </c>
       <c r="C6" s="7">
-        <v>43476</v>
+        <v>43535</v>
       </c>
       <c r="D6" s="7">
-        <v>43476</v>
+        <v>43535</v>
       </c>
       <c r="E6" s="10">
         <f t="shared" si="0"/>
-        <v>1547164800</v>
+        <v>1552262400</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="H6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I6" t="s">
         <v>13</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="323" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7" s="7">
-        <v>43535</v>
+        <v>43516</v>
       </c>
       <c r="D7" s="7">
-        <v>43535</v>
+        <v>43518</v>
       </c>
       <c r="E7" s="10">
         <f t="shared" si="0"/>
-        <v>1552262400</v>
+        <v>1550620800</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>45</v>
@@ -910,164 +898,132 @@
         <v>46</v>
       </c>
       <c r="H7" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I7" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="323" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C8" s="7">
-        <v>43516</v>
+        <v>43489</v>
       </c>
       <c r="D8" s="7">
-        <v>43518</v>
+        <v>43489</v>
       </c>
       <c r="E8" s="10">
         <f t="shared" si="0"/>
-        <v>1550620800</v>
+        <v>1548288000</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="H8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I8" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C9" s="7">
-        <v>43481</v>
+        <v>43625</v>
       </c>
       <c r="D9" s="7">
-        <v>43481</v>
+        <v>43630</v>
       </c>
       <c r="E9" s="10">
         <f t="shared" si="0"/>
-        <v>1547596800</v>
+        <v>1560038400</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>54</v>
+        <v>63</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>62</v>
       </c>
       <c r="H9" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="I9" t="s">
         <v>13</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="388" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C10" s="7">
-        <v>43481</v>
+        <v>43509</v>
       </c>
       <c r="D10" s="7">
-        <v>43481</v>
+        <v>43509</v>
       </c>
       <c r="E10" s="10">
         <f t="shared" si="0"/>
-        <v>1547596800</v>
+        <v>1550016000</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="H10" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="I10" t="s">
         <v>25</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="68" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="7">
-        <v>43489</v>
-      </c>
-      <c r="D11" s="7">
-        <v>43489</v>
-      </c>
-      <c r="E11" s="10">
-        <f t="shared" si="0"/>
-        <v>1548288000</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="H11" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" xr:uid="{1E644AB0-1CE4-CA43-BC4B-C485696BC585}"/>
     <hyperlink ref="G4" r:id="rId2" xr:uid="{435D4641-689C-4342-BC3A-BE8C2BA92CAC}"/>
-    <hyperlink ref="G11" r:id="rId3" xr:uid="{7061BBBD-8C92-C44E-81EC-A5D1BFE78C35}"/>
+    <hyperlink ref="G8" r:id="rId3" xr:uid="{7061BBBD-8C92-C44E-81EC-A5D1BFE78C35}"/>
+    <hyperlink ref="G9" r:id="rId4" xr:uid="{0EF61B36-07A0-E64B-969C-AA716B3488A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Removed old events and added new NIH Library events
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D711551-96B2-DD4E-A9BE-5E6C0BDFB964}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B305436E-0751-3F49-9C43-928D18E823AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22720" yWindow="600" windowWidth="27580" windowHeight="19740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="81">
   <si>
     <t>type</t>
   </si>
@@ -188,27 +188,9 @@
     <t>statistics,data analysis,R</t>
   </si>
   <si>
-    <t>NICBR Winter Symposium "Novel Therapeutics"</t>
-  </si>
-  <si>
     <t>MICROBIOME listserv</t>
   </si>
   <si>
-    <t>National Cancer Institute at Frederick, Bldg. 549</t>
-  </si>
-  <si>
-    <t>https://ncifrederick.cancer.gov/events/conferences/nicbr-winter-symposium-novel-therapeutics</t>
-  </si>
-  <si>
-    <t>Symposium</t>
-  </si>
-  <si>
-    <t>This symposium will feature talks from the Frederick research community on novel therapeutics for infectious diseases, cancer and autoimmunity.</t>
-  </si>
-  <si>
-    <t>antibiotic-resistant bacteria,natural product modulators,personalized therapies</t>
-  </si>
-  <si>
     <t>https://ncbiinsights.ncbi.nlm.nih.gov/2018/12/20/suggest-project-nih-biodata-hackathon/</t>
   </si>
   <si>
@@ -249,18 +231,6 @@
   </si>
   <si>
     <t>Online only</t>
-  </si>
-  <si>
-    <t>Consortium on Translational Research in the Microbiome</t>
-  </si>
-  <si>
-    <t>https://www.westchesterbiotechproject.org/microbiome-ctrm</t>
-  </si>
-  <si>
-    <t>This ongoing Roundtable addresses data generation, collection, sequencing, analysis, and harmonizing systems to accelerate relevant, reproducible research. After briefs from our speakers, you’ll be invited to introduce yourself and your venue (institute or industry). This is your opportunity to discuss best practices and lessons learned with your peers.</t>
-  </si>
-  <si>
-    <t>DNA extraction,reproducibility,data analytics</t>
   </si>
   <si>
     <t>Informatics for Precision Medicine
@@ -277,6 +247,42 @@
   </si>
   <si>
     <t>data integration,RNA biology,genomics,drug discovery,ontology,visualization</t>
+  </si>
+  <si>
+    <t>Data Wrangling in R</t>
+  </si>
+  <si>
+    <t>NIH Library Training Room</t>
+  </si>
+  <si>
+    <t>https://www.nihlibrary.nih.gov/training/data-wrangling-r</t>
+  </si>
+  <si>
+    <t>R is a programming language and open source environment for statistical computing and graphics. The R series is a comprehensive collection of training sessions designed to teach non-programmers how to write modular code and to introduce best practices for using R for data analysis and data visualization. Each class uses both evidence-based best practices for programming and practical hands-on lessons. In this two-hour class, participants will be provided a basic overview of manipulating, analyzing and exporting data using the R tidyverse. Participants will leave the course with a better understanding of how to better manage data for more efficient and effective analysis.</t>
+  </si>
+  <si>
+    <t>open source,R,data analysis,data visualization</t>
+  </si>
+  <si>
+    <t>Data Visualization in R in ggplot</t>
+  </si>
+  <si>
+    <t>https://www.nihlibrary.nih.gov/training/data-visualization-r-ggplot</t>
+  </si>
+  <si>
+    <t>R is a programming language and open source environment for statistical computing and graphics. The R series is a comprehensive collection of training sessions designed to teach non-programmers how to write modular code and to introduce best practices for using R for data analysis and data visualization. Each class uses both evidence-based best practices for programming and practical hands-on lessons. This class provides a basic overview of using R to create data visualizations. Participants will become familiar with using R to produce scatter plots, boxplots, and time series plots using ggplot.</t>
+  </si>
+  <si>
+    <t>Statistical Methods for Complex Sample Survey Data Analysis</t>
+  </si>
+  <si>
+    <t>https://www.nihlibrary.nih.gov/training/statistical-methods-complex-sample-survey-data-analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Questionnaires and surveys are widely used tools for collecting research data, and analytical methods for these tools are varied and depend on many design factors. Participants in this two-hour intermediate level class will learn the valid methods of analysis for complex sample survey data. Specifically, participants will gain knowledge in variance estimation methods and contrast results between model-based and design-based statistical approaches. This class will provide participants with an overview of complex survey design features and the data analysis process for these surveys, from hypothesis formulation to statistical inference, including design effects and weighting, exploratory data analysis, variables selection, variance estimation methods, and model selection.  This hands-on experience uses real survey data in SAS to demonstrate the steps and techniques. Participants should have a basic understanding of SAS, probabilities, sampling, and linear/logistic regression to fully benefit from the class. </t>
+  </si>
+  <si>
+    <t>sample survey data,variance estimation,statistics</t>
   </si>
 </sst>
 </file>
@@ -666,11 +672,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -775,7 +781,7 @@
         <v>43642</v>
       </c>
       <c r="E3" s="10">
-        <f t="shared" ref="E3:E12" si="0">(C3-DATE(1970,1,1))*86400</f>
+        <f t="shared" ref="E3:E13" si="0">(C3-DATE(1970,1,1))*86400</f>
         <v>1561420800</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -848,10 +854,10 @@
         <v>1550620800</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H5" t="s">
         <v>36</v>
@@ -938,31 +944,31 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C8" s="7">
-        <v>43489</v>
+        <v>43625</v>
       </c>
       <c r="D8" s="7">
-        <v>43489</v>
+        <v>43630</v>
       </c>
       <c r="E8" s="10">
         <f t="shared" si="0"/>
-        <v>1548288000</v>
+        <v>1560038400</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="I8" t="s">
         <v>13</v>
@@ -974,70 +980,70 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="7">
-        <v>43625</v>
+        <v>43509</v>
       </c>
       <c r="D9" s="7">
-        <v>43630</v>
+        <v>43509</v>
       </c>
       <c r="E9" s="10">
         <f t="shared" si="0"/>
-        <v>1560038400</v>
+        <v>1550016000</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:12" ht="136" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>64</v>
       </c>
       <c r="C10" s="7">
-        <v>43509</v>
+        <v>43552</v>
       </c>
       <c r="D10" s="7">
-        <v>43509</v>
+        <v>43554</v>
       </c>
       <c r="E10" s="10">
         <f t="shared" si="0"/>
-        <v>1550016000</v>
+        <v>1553731200</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="I10" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>67</v>
@@ -1046,34 +1052,34 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C11" s="7">
-        <v>43490</v>
+        <v>43501</v>
       </c>
       <c r="D11" s="7">
-        <v>43490</v>
+        <v>43501</v>
       </c>
       <c r="E11" s="10">
         <f t="shared" si="0"/>
-        <v>1548374400</v>
+        <v>1549324800</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>71</v>
       </c>
       <c r="H11" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="I11" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>72</v>
@@ -1082,7 +1088,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>14</v>
       </c>
@@ -1090,40 +1096,75 @@
         <v>74</v>
       </c>
       <c r="C12" s="7">
-        <v>43552</v>
+        <v>43515</v>
       </c>
       <c r="D12" s="7">
-        <v>43554</v>
+        <v>43515</v>
       </c>
       <c r="E12" s="10">
         <f t="shared" si="0"/>
-        <v>1553731200</v>
+        <v>1550534400</v>
       </c>
       <c r="F12" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>76</v>
-      </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="I12" t="s">
         <v>13</v>
       </c>
       <c r="J12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="C13" s="7">
+        <v>43524</v>
+      </c>
+      <c r="D13" s="7">
+        <v>43524</v>
+      </c>
+      <c r="E13" s="10">
+        <f t="shared" si="0"/>
+        <v>1551312000</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>78</v>
+      </c>
+      <c r="H13" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" xr:uid="{1E644AB0-1CE4-CA43-BC4B-C485696BC585}"/>
     <hyperlink ref="G4" r:id="rId2" xr:uid="{435D4641-689C-4342-BC3A-BE8C2BA92CAC}"/>
-    <hyperlink ref="G8" r:id="rId3" xr:uid="{7061BBBD-8C92-C44E-81EC-A5D1BFE78C35}"/>
-    <hyperlink ref="G9" r:id="rId4" xr:uid="{0EF61B36-07A0-E64B-969C-AA716B3488A5}"/>
+    <hyperlink ref="G8" r:id="rId3" xr:uid="{0EF61B36-07A0-E64B-969C-AA716B3488A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Updated with BCBB seminars
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B305436E-0751-3F49-9C43-928D18E823AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A68BFC-9855-4A47-892C-91DC99A8AE6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22720" yWindow="600" windowWidth="27580" windowHeight="19740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27780" yWindow="460" windowWidth="27580" windowHeight="19740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="103">
   <si>
     <t>type</t>
   </si>
@@ -283,6 +283,75 @@
   </si>
   <si>
     <t>sample survey data,variance estimation,statistics</t>
+  </si>
+  <si>
+    <t>Programmer's Corner: Database Design</t>
+  </si>
+  <si>
+    <t>Bldg 549 Rm B</t>
+  </si>
+  <si>
+    <t>https://cbiit.webex.com/cbiit/j.php?MTID=maaa477c0a365f5eb9fa07dcdb913200a</t>
+  </si>
+  <si>
+    <t>Organizing and managing data is critical for developing any application. What is involved in designing and setting up a new database? The presentation will cover the different terms and types of SQL and NoSQL databases, aspects to consider before choosing a specific data management system for any research project and support offered for the NCI community.
+Examples and use cases will be presented that demonstrate how SQL and NoSQL database back-ends were chosen for specific research applications.</t>
+  </si>
+  <si>
+    <t>database,SQL,NoSQL</t>
+  </si>
+  <si>
+    <t>Microbial networking (…it's like Tinder for bugs)</t>
+  </si>
+  <si>
+    <t>NIH-STAFF listserv</t>
+  </si>
+  <si>
+    <t>NIH Main Campus, Building 10, Masur Auditorium</t>
+  </si>
+  <si>
+    <t>Lecture</t>
+  </si>
+  <si>
+    <t>Few microbes (viruses, bacteria, fungi) live in isolation or exclusively with members of their own kingdom or domain. Affinities or aversions among microbial members influence the community structure, but these interactions can be reorganized with the arrival of disruptors. In respiratory infections, for example, infectious agents—be they viral or bacterial—are entering an environment within the host where they can impact existing ecological relationships among local residents. Disrupting these "social" networks has ecological and physiological consequences.
+As we begin to discover the importance of microbial associations in understanding host-pathogen interactions, we need innovative ways to capture direct and indirect effects between viruses, fungi, bacteria, and the host. However, determining if microbes are "swiping left or swiping right" is challenging from an analytical perspective as most ecological interaction networks do not reach much beyond their own kingdom.
+For her lecture, Dr. Ghedin will discuss some of her laboratory's work on respiratory tract infections, such as tuberculosis and influenza, and how her lab tackles the complex host-pathogen interplay by inferring networks of interactions among microbes and with their hosts.</t>
+  </si>
+  <si>
+    <t>microbe,associations</t>
+  </si>
+  <si>
+    <t>NIAID BioIT listserv</t>
+  </si>
+  <si>
+    <t>Unix for Biologists</t>
+  </si>
+  <si>
+    <t>NIH Main Campus, Building 3, Room 3/1E14</t>
+  </si>
+  <si>
+    <t>http://www.eventzilla.net/user/NIAID_OCICB_BCBB</t>
+  </si>
+  <si>
+    <t>This course will help participants with no computational background to get started using Unix for analytical tasks. After completing the training the participants should be able to confidently use the command line interface on either a local (laptop) or remote (cluster) Unix system and to navigate around the Unix file system from the command line, use a number of common Unix commands and create basic Unix scripts. The course will include a mix of lecture and hands-on components.</t>
+  </si>
+  <si>
+    <t>Unix,command line</t>
+  </si>
+  <si>
+    <t>Determining the effect of a mutation in a protein structure using computational biology</t>
+  </si>
+  <si>
+    <t>This workshop will seek to equip you with the tools necessary to begin answering two of the more common questions in computational structural biology – how do I model a structure and determine the effect of a mutation on the stability of my protein?  Topics to be addressed will be molecular visualization including virtual reality, homology modeling, free energy calculations, and protein-ligand docking.  The workshop will contain a mix of lecture and hands-on components, and will be immediately preceded by a short introductory course on Unix and cluster computing.</t>
+  </si>
+  <si>
+    <t>structural biology,modeling,mutation</t>
+  </si>
+  <si>
+    <t>Determining the effect of a mutation in a protein structure using computational biology – Part 2</t>
+  </si>
+  <si>
+    <t>Determining the effect of a mutation in a protein structure using computational biology – Part 3</t>
   </si>
 </sst>
 </file>
@@ -672,11 +741,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -781,7 +850,7 @@
         <v>43642</v>
       </c>
       <c r="E3" s="10">
-        <f t="shared" ref="E3:E13" si="0">(C3-DATE(1970,1,1))*86400</f>
+        <f t="shared" ref="E3:E19" si="0">(C3-DATE(1970,1,1))*86400</f>
         <v>1561420800</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -1158,6 +1227,219 @@
       </c>
       <c r="K13" s="9" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="7">
+        <v>43503</v>
+      </c>
+      <c r="D14" s="7">
+        <v>43503</v>
+      </c>
+      <c r="E14" s="10">
+        <f t="shared" si="0"/>
+        <v>1549497600</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="7">
+        <v>43502</v>
+      </c>
+      <c r="D15" s="7">
+        <v>43502</v>
+      </c>
+      <c r="E15" s="10">
+        <f t="shared" si="0"/>
+        <v>1549411200</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15" t="s">
+        <v>89</v>
+      </c>
+      <c r="I15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="7">
+        <v>43522</v>
+      </c>
+      <c r="D16" s="7">
+        <v>43522</v>
+      </c>
+      <c r="E16" s="10">
+        <f t="shared" si="0"/>
+        <v>1551139200</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="7">
+        <v>43522</v>
+      </c>
+      <c r="D17" s="7">
+        <v>43522</v>
+      </c>
+      <c r="E17" s="10">
+        <f t="shared" si="0"/>
+        <v>1551139200</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="7">
+        <v>43523</v>
+      </c>
+      <c r="D18" s="7">
+        <v>43523</v>
+      </c>
+      <c r="E18" s="10">
+        <f t="shared" si="0"/>
+        <v>1551225600</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="7">
+        <v>43524</v>
+      </c>
+      <c r="D19" s="7">
+        <v>43524</v>
+      </c>
+      <c r="E19" s="10">
+        <f t="shared" si="0"/>
+        <v>1551312000</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
delete events from last week
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/booirizarryy/Desktop/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A68BFC-9855-4A47-892C-91DC99A8AE6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CFF1EF-C052-E249-9068-02B01568E18A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27780" yWindow="460" windowWidth="27580" windowHeight="19740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1220" yWindow="460" windowWidth="27580" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="89">
   <si>
     <t>type</t>
   </si>
@@ -233,10 +233,6 @@
     <t>Online only</t>
   </si>
   <si>
-    <t>Informatics for Precision Medicine
-16th Annual Conference of the Midsouth Computational Biology &amp; Bioinformatics Society (MCBIOS ’19)</t>
-  </si>
-  <si>
     <t>Hilton Birmingham at UAB 808 20th Street South, Birmingham, AL 35205</t>
   </si>
   <si>
@@ -249,18 +245,9 @@
     <t>data integration,RNA biology,genomics,drug discovery,ontology,visualization</t>
   </si>
   <si>
-    <t>Data Wrangling in R</t>
-  </si>
-  <si>
     <t>NIH Library Training Room</t>
   </si>
   <si>
-    <t>https://www.nihlibrary.nih.gov/training/data-wrangling-r</t>
-  </si>
-  <si>
-    <t>R is a programming language and open source environment for statistical computing and graphics. The R series is a comprehensive collection of training sessions designed to teach non-programmers how to write modular code and to introduce best practices for using R for data analysis and data visualization. Each class uses both evidence-based best practices for programming and practical hands-on lessons. In this two-hour class, participants will be provided a basic overview of manipulating, analyzing and exporting data using the R tidyverse. Participants will leave the course with a better understanding of how to better manage data for more efficient and effective analysis.</t>
-  </si>
-  <si>
     <t>open source,R,data analysis,data visualization</t>
   </si>
   <si>
@@ -285,42 +272,6 @@
     <t>sample survey data,variance estimation,statistics</t>
   </si>
   <si>
-    <t>Programmer's Corner: Database Design</t>
-  </si>
-  <si>
-    <t>Bldg 549 Rm B</t>
-  </si>
-  <si>
-    <t>https://cbiit.webex.com/cbiit/j.php?MTID=maaa477c0a365f5eb9fa07dcdb913200a</t>
-  </si>
-  <si>
-    <t>Organizing and managing data is critical for developing any application. What is involved in designing and setting up a new database? The presentation will cover the different terms and types of SQL and NoSQL databases, aspects to consider before choosing a specific data management system for any research project and support offered for the NCI community.
-Examples and use cases will be presented that demonstrate how SQL and NoSQL database back-ends were chosen for specific research applications.</t>
-  </si>
-  <si>
-    <t>database,SQL,NoSQL</t>
-  </si>
-  <si>
-    <t>Microbial networking (…it's like Tinder for bugs)</t>
-  </si>
-  <si>
-    <t>NIH-STAFF listserv</t>
-  </si>
-  <si>
-    <t>NIH Main Campus, Building 10, Masur Auditorium</t>
-  </si>
-  <si>
-    <t>Lecture</t>
-  </si>
-  <si>
-    <t>Few microbes (viruses, bacteria, fungi) live in isolation or exclusively with members of their own kingdom or domain. Affinities or aversions among microbial members influence the community structure, but these interactions can be reorganized with the arrival of disruptors. In respiratory infections, for example, infectious agents—be they viral or bacterial—are entering an environment within the host where they can impact existing ecological relationships among local residents. Disrupting these "social" networks has ecological and physiological consequences.
-As we begin to discover the importance of microbial associations in understanding host-pathogen interactions, we need innovative ways to capture direct and indirect effects between viruses, fungi, bacteria, and the host. However, determining if microbes are "swiping left or swiping right" is challenging from an analytical perspective as most ecological interaction networks do not reach much beyond their own kingdom.
-For her lecture, Dr. Ghedin will discuss some of her laboratory's work on respiratory tract infections, such as tuberculosis and influenza, and how her lab tackles the complex host-pathogen interplay by inferring networks of interactions among microbes and with their hosts.</t>
-  </si>
-  <si>
-    <t>microbe,associations</t>
-  </si>
-  <si>
     <t>NIAID BioIT listserv</t>
   </si>
   <si>
@@ -352,6 +303,9 @@
   </si>
   <si>
     <t>Determining the effect of a mutation in a protein structure using computational biology – Part 3</t>
+  </si>
+  <si>
+    <t>Informatics for Precision Medicine 16th Annual Conference of the Midsouth Computational Biology &amp; Bioinformatics Society (MCBIOS ’19)</t>
   </si>
 </sst>
 </file>
@@ -741,11 +695,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -799,118 +753,120 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="12">
-        <v>43537</v>
-      </c>
-      <c r="D2" s="12">
-        <v>43540</v>
+        <v>49</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="7">
+        <v>43509</v>
+      </c>
+      <c r="D2" s="7">
+        <v>43509</v>
       </c>
       <c r="E2" s="10">
         <f>(C2-DATE(1970,1,1))*86400</f>
-        <v>1552435200</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="14"/>
-    </row>
-    <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>1550016000</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="C3" s="7">
-        <v>43641</v>
+        <v>43515</v>
       </c>
       <c r="D3" s="7">
-        <v>43642</v>
+        <v>43515</v>
       </c>
       <c r="E3" s="10">
-        <f t="shared" ref="E3:E19" si="0">(C3-DATE(1970,1,1))*86400</f>
-        <v>1561420800</v>
+        <f>(C3-DATE(1970,1,1))*86400</f>
+        <v>1550534400</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" t="s">
         <v>13</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="187" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C4" s="7">
-        <v>43535</v>
+        <v>43516</v>
       </c>
       <c r="D4" s="7">
-        <v>43541</v>
+        <v>43518</v>
       </c>
       <c r="E4" s="10">
-        <f t="shared" si="0"/>
-        <v>1552262400</v>
+        <f>(C4-DATE(1970,1,1))*86400</f>
+        <v>1550620800</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>30</v>
+        <v>51</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>50</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="I4" t="s">
         <v>13</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="323" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C5" s="7">
         <v>43516</v>
@@ -919,206 +875,206 @@
         <v>43518</v>
       </c>
       <c r="E5" s="10">
-        <f t="shared" si="0"/>
+        <f>(C5-DATE(1970,1,1))*86400</f>
         <v>1550620800</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>50</v>
+        <v>45</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="C6" s="7">
-        <v>43535</v>
+        <v>43522</v>
       </c>
       <c r="D6" s="7">
-        <v>43535</v>
+        <v>43522</v>
       </c>
       <c r="E6" s="10">
-        <f t="shared" si="0"/>
-        <v>1552262400</v>
+        <f>(C6-DATE(1970,1,1))*86400</f>
+        <v>1551139200</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="H6" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="I6" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="323" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="C7" s="7">
-        <v>43516</v>
+        <v>43522</v>
       </c>
       <c r="D7" s="7">
-        <v>43518</v>
+        <v>43522</v>
       </c>
       <c r="E7" s="10">
-        <f t="shared" si="0"/>
-        <v>1550620800</v>
+        <f>(C7-DATE(1970,1,1))*86400</f>
+        <v>1551139200</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="H7" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="I7" t="s">
         <v>25</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="C8" s="7">
-        <v>43625</v>
+        <v>43523</v>
       </c>
       <c r="D8" s="7">
-        <v>43630</v>
+        <v>43523</v>
       </c>
       <c r="E8" s="10">
-        <f t="shared" si="0"/>
-        <v>1560038400</v>
+        <f>(C8-DATE(1970,1,1))*86400</f>
+        <v>1551225600</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>56</v>
+        <v>79</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
       </c>
       <c r="I8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="7">
+        <v>43524</v>
+      </c>
+      <c r="D9" s="7">
+        <v>43524</v>
+      </c>
+      <c r="E9" s="10">
+        <f>(C9-DATE(1970,1,1))*86400</f>
+        <v>1551312000</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="119" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="7">
-        <v>43509</v>
-      </c>
-      <c r="D9" s="7">
-        <v>43509</v>
-      </c>
-      <c r="E9" s="10">
-        <f t="shared" si="0"/>
-        <v>1550016000</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="H9" t="s">
-        <v>60</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="J9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="7">
+        <v>43524</v>
+      </c>
+      <c r="D10" s="7">
+        <v>43524</v>
+      </c>
+      <c r="E10" s="10">
+        <f>(C10-DATE(1970,1,1))*86400</f>
+        <v>1551312000</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="136" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="7">
-        <v>43552</v>
-      </c>
-      <c r="D10" s="7">
-        <v>43554</v>
-      </c>
-      <c r="E10" s="10">
-        <f t="shared" si="0"/>
-        <v>1553731200</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" t="s">
-        <v>13</v>
-      </c>
       <c r="J10" s="3" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="102" x14ac:dyDescent="0.2">
@@ -1126,327 +1082,223 @@
         <v>14</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="C11" s="7">
-        <v>43501</v>
+        <v>43535</v>
       </c>
       <c r="D11" s="7">
-        <v>43501</v>
+        <v>43541</v>
       </c>
       <c r="E11" s="10">
-        <f t="shared" si="0"/>
-        <v>1549324800</v>
+        <f>(C11-DATE(1970,1,1))*86400</f>
+        <v>1552262400</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>71</v>
+        <v>31</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>30</v>
       </c>
       <c r="H11" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="I11" t="s">
         <v>13</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="C12" s="7">
-        <v>43515</v>
+        <v>43535</v>
       </c>
       <c r="D12" s="7">
-        <v>43515</v>
+        <v>43535</v>
       </c>
       <c r="E12" s="10">
-        <f t="shared" si="0"/>
-        <v>1550534400</v>
+        <f>(C12-DATE(1970,1,1))*86400</f>
+        <v>1552262400</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="H12" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I12" t="s">
         <v>13</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C13" s="7">
-        <v>43524</v>
-      </c>
-      <c r="D13" s="7">
-        <v>43524</v>
+        <v>12</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="12">
+        <v>43537</v>
+      </c>
+      <c r="D13" s="12">
+        <v>43540</v>
       </c>
       <c r="E13" s="10">
-        <f t="shared" si="0"/>
-        <v>1551312000</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="H13" t="s">
-        <v>47</v>
-      </c>
-      <c r="I13" t="s">
+        <f>(C13-DATE(1970,1,1))*86400</f>
+        <v>1552435200</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+      <c r="J13" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="14"/>
+    </row>
+    <row r="14" spans="1:12" ht="136" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C14" s="7">
-        <v>43503</v>
+        <v>43552</v>
       </c>
       <c r="D14" s="7">
-        <v>43503</v>
+        <v>43554</v>
       </c>
       <c r="E14" s="10">
-        <f t="shared" si="0"/>
-        <v>1549497600</v>
+        <f>(C14-DATE(1970,1,1))*86400</f>
+        <v>1553731200</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="H14" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="I14" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="C15" s="7">
-        <v>43502</v>
+        <v>43625</v>
       </c>
       <c r="D15" s="7">
-        <v>43502</v>
+        <v>43630</v>
       </c>
       <c r="E15" s="10">
-        <f t="shared" si="0"/>
-        <v>1549411200</v>
+        <f>(C15-DATE(1970,1,1))*86400</f>
+        <v>1560038400</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>88</v>
+        <v>57</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="H15" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="I15" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>93</v>
+        <v>23</v>
       </c>
       <c r="C16" s="7">
-        <v>43522</v>
+        <v>43641</v>
       </c>
       <c r="D16" s="7">
-        <v>43522</v>
+        <v>43642</v>
       </c>
       <c r="E16" s="10">
-        <f t="shared" si="0"/>
-        <v>1551139200</v>
+        <f>(C16-DATE(1970,1,1))*86400</f>
+        <v>1561420800</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="H16" t="s">
-        <v>47</v>
-      </c>
-      <c r="I16" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" s="7">
-        <v>43522</v>
-      </c>
-      <c r="D17" s="7">
-        <v>43522</v>
-      </c>
-      <c r="E17" s="10">
-        <f t="shared" si="0"/>
-        <v>1551139200</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="H17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="K17" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="7">
-        <v>43523</v>
-      </c>
-      <c r="D18" s="7">
-        <v>43523</v>
-      </c>
-      <c r="E18" s="10">
-        <f t="shared" si="0"/>
-        <v>1551225600</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="H18" t="s">
-        <v>20</v>
-      </c>
-      <c r="I18" t="s">
-        <v>25</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C19" s="7">
-        <v>43524</v>
-      </c>
-      <c r="D19" s="7">
-        <v>43524</v>
-      </c>
-      <c r="E19" s="10">
-        <f t="shared" si="0"/>
-        <v>1551312000</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="H19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I19" t="s">
-        <v>25</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="K19" s="9" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:L17">
+    <sortCondition ref="C1"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" xr:uid="{1E644AB0-1CE4-CA43-BC4B-C485696BC585}"/>
-    <hyperlink ref="G4" r:id="rId2" xr:uid="{435D4641-689C-4342-BC3A-BE8C2BA92CAC}"/>
-    <hyperlink ref="G8" r:id="rId3" xr:uid="{0EF61B36-07A0-E64B-969C-AA716B3488A5}"/>
+    <hyperlink ref="G16" r:id="rId1" xr:uid="{1E644AB0-1CE4-CA43-BC4B-C485696BC585}"/>
+    <hyperlink ref="G11" r:id="rId2" xr:uid="{435D4641-689C-4342-BC3A-BE8C2BA92CAC}"/>
+    <hyperlink ref="G15" r:id="rId3" xr:uid="{0EF61B36-07A0-E64B-969C-AA716B3488A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Updated with new entries 2/19
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/booirizarryy/Desktop/nbp_events_niaid/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CFF1EF-C052-E249-9068-02B01568E18A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96ED7CF-03EB-0E48-A636-9FC8E065A32E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="460" windowWidth="27580" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6760" yWindow="8560" windowWidth="27580" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="89">
   <si>
     <t>type</t>
   </si>
@@ -188,9 +188,6 @@
     <t>statistics,data analysis,R</t>
   </si>
   <si>
-    <t>MICROBIOME listserv</t>
-  </si>
-  <si>
     <t>https://ncbiinsights.ncbi.nlm.nih.gov/2018/12/20/suggest-project-nih-biodata-hackathon/</t>
   </si>
   <si>
@@ -215,24 +212,6 @@
     <t>Oak Ridge National Laboratory, 8640 Nano Center Drive Oak Ridge, TN 37830</t>
   </si>
   <si>
-    <t>Generating High-quality Genome Drafts from Uncultured Microbiome Samples with a Single Shotgun Experiment</t>
-  </si>
-  <si>
-    <t>https://www.10xgenomics.com/event/generating-high-quality-genome-drafts-from-uncultured-microbiome-samples/</t>
-  </si>
-  <si>
-    <t>Webinar</t>
-  </si>
-  <si>
-    <t>This webinar will feature a presentation on a recently published method for de novo assembly of microbial genome drafts using short read sequencing. The method uses Chromium Linked-Read sequencing and a novel computational analysis pipeline, Athena, to construct high-quality microbial genome drafts of metagenomic communities sampled directly from their environments. In uncultured samples from human stool, Athena produced individual genome drafts with high contiguity (&gt;200-kb N50, fewer than ten contigs), even for bacteria with relatively low raw short-read sequence coverage. Compared with results from existing short-read and synthetic long-read metagenomic sequencing techniques, the Athena assemblies are the most contiguous reported to date.</t>
-  </si>
-  <si>
-    <t>de novo assembly,Athena,short-read sequencing</t>
-  </si>
-  <si>
-    <t>Online only</t>
-  </si>
-  <si>
     <t>Hilton Birmingham at UAB 808 20th Street South, Birmingham, AL 35205</t>
   </si>
   <si>
@@ -306,6 +285,28 @@
   </si>
   <si>
     <t>Informatics for Precision Medicine 16th Annual Conference of the Midsouth Computational Biology &amp; Bioinformatics Society (MCBIOS ’19)</t>
+  </si>
+  <si>
+    <t>A Hole New View: Structure-Function Mapping of the Nuclear Pore Complex</t>
+  </si>
+  <si>
+    <t>NIH Main Campus, Building 35, Room 640</t>
+  </si>
+  <si>
+    <t>mapping</t>
+  </si>
+  <si>
+    <t>Electronic Lab Notebook Forum</t>
+  </si>
+  <si>
+    <t>Do you use an electronic lab notebook (ELN), or are you interested in implementing one for your lab? Join us for an Electronic Lab Notebook Forum on Monday, March 11, 9:00 a.m.-2:00 p.m. in Lipsett Amphitheater, Building 10.
+Organized by the NIH Library, this one-day event will focus on exploring the benefits and challenges of ELN implementation and use. The program begins with a series of case studies on ELNs presented by Hivebench, LabArchives, Labguru, and PerkinElmer in partnership with NIH intramural researchers. After a break, the event continues with lightning talks on topics related to ELN implementation, administration, usability, and functionality. The program concludes with a Q&amp;A session and closing remarks.</t>
+  </si>
+  <si>
+    <t>electronic lab notebook,ELN</t>
+  </si>
+  <si>
+    <t>https://www.nihlibrary.nih.gov/eln-forum</t>
   </si>
 </sst>
 </file>
@@ -695,11 +696,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -753,84 +754,84 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C2" s="7">
-        <v>43509</v>
+        <v>43515</v>
       </c>
       <c r="D2" s="7">
-        <v>43509</v>
+        <v>43515</v>
       </c>
       <c r="E2" s="10">
-        <f>(C2-DATE(1970,1,1))*86400</f>
-        <v>1550016000</v>
+        <f t="shared" ref="E2:E17" si="0">(C2-DATE(1970,1,1))*86400</f>
+        <v>1550534400</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="187" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="C3" s="7">
-        <v>43515</v>
+        <v>43516</v>
       </c>
       <c r="D3" s="7">
-        <v>43515</v>
+        <v>43518</v>
       </c>
       <c r="E3" s="10">
-        <f>(C3-DATE(1970,1,1))*86400</f>
-        <v>1550534400</v>
+        <f t="shared" si="0"/>
+        <v>1550620800</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>71</v>
+        <v>50</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>49</v>
       </c>
       <c r="H3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="I3" t="s">
         <v>13</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="323" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C4" s="7">
         <v>43516</v>
@@ -839,50 +840,50 @@
         <v>43518</v>
       </c>
       <c r="E4" s="10">
-        <f>(C4-DATE(1970,1,1))*86400</f>
+        <f t="shared" si="0"/>
         <v>1550620800</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>50</v>
+        <v>45</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="H4" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="I4" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="323" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="C5" s="7">
-        <v>43516</v>
+        <v>43522</v>
       </c>
       <c r="D5" s="7">
-        <v>43518</v>
+        <v>43522</v>
       </c>
       <c r="E5" s="10">
-        <f>(C5-DATE(1970,1,1))*86400</f>
-        <v>1550620800</v>
+        <f t="shared" si="0"/>
+        <v>1551139200</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="H5" t="s">
         <v>47</v>
@@ -891,18 +892,18 @@
         <v>25</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C6" s="7">
         <v>43522</v>
@@ -911,50 +912,50 @@
         <v>43522</v>
       </c>
       <c r="E6" s="10">
-        <f>(C6-DATE(1970,1,1))*86400</f>
+        <f t="shared" si="0"/>
         <v>1551139200</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="I6" t="s">
         <v>25</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C7" s="7">
-        <v>43522</v>
+        <v>43523</v>
       </c>
       <c r="D7" s="7">
-        <v>43522</v>
+        <v>43523</v>
       </c>
       <c r="E7" s="10">
-        <f>(C7-DATE(1970,1,1))*86400</f>
-        <v>1551139200</v>
+        <f t="shared" si="0"/>
+        <v>1551225600</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="H7" t="s">
         <v>20</v>
@@ -963,54 +964,54 @@
         <v>25</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="153" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="C8" s="7">
-        <v>43523</v>
+        <v>43524</v>
       </c>
       <c r="D8" s="7">
-        <v>43523</v>
+        <v>43524</v>
       </c>
       <c r="E8" s="10">
-        <f>(C8-DATE(1970,1,1))*86400</f>
-        <v>1551225600</v>
+        <f t="shared" si="0"/>
+        <v>1551312000</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="G8" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="H8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="153" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>73</v>
       </c>
       <c r="C9" s="7">
         <v>43524</v>
@@ -1019,286 +1020,316 @@
         <v>43524</v>
       </c>
       <c r="E9" s="10">
-        <f>(C9-DATE(1970,1,1))*86400</f>
+        <f t="shared" si="0"/>
         <v>1551312000</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H9" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="I9" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
       <c r="C10" s="7">
-        <v>43524</v>
+        <v>43535</v>
       </c>
       <c r="D10" s="7">
-        <v>43524</v>
+        <v>43541</v>
       </c>
       <c r="E10" s="10">
-        <f>(C10-DATE(1970,1,1))*86400</f>
-        <v>1551312000</v>
+        <f t="shared" si="0"/>
+        <v>1552262400</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>80</v>
+        <v>31</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>30</v>
       </c>
       <c r="H10" t="s">
         <v>20</v>
       </c>
       <c r="I10" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>85</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C11" s="7">
         <v>43535</v>
       </c>
       <c r="D11" s="7">
-        <v>43541</v>
+        <v>43535</v>
       </c>
       <c r="E11" s="10">
-        <f>(C11-DATE(1970,1,1))*86400</f>
+        <f t="shared" si="0"/>
         <v>1552262400</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>30</v>
+        <v>41</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="H11" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="I11" t="s">
         <v>13</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="7">
-        <v>43535</v>
-      </c>
-      <c r="D12" s="7">
-        <v>43535</v>
+        <v>12</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="12">
+        <v>43537</v>
+      </c>
+      <c r="D12" s="12">
+        <v>43540</v>
       </c>
       <c r="E12" s="10">
-        <f>(C12-DATE(1970,1,1))*86400</f>
-        <v>1552262400</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="H12" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" t="s">
+        <f t="shared" si="0"/>
+        <v>1552435200</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="J12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="14"/>
+    </row>
+    <row r="13" spans="1:12" ht="136" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="12">
-        <v>43537</v>
-      </c>
-      <c r="D13" s="12">
-        <v>43540</v>
+        <v>14</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="7">
+        <v>43552</v>
+      </c>
+      <c r="D13" s="7">
+        <v>43554</v>
       </c>
       <c r="E13" s="10">
-        <f>(C13-DATE(1970,1,1))*86400</f>
-        <v>1552435200</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="10" t="s">
+        <f t="shared" si="0"/>
+        <v>1553731200</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" t="s">
         <v>15</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I13" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L13" s="14"/>
-    </row>
-    <row r="14" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+      <c r="J13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="C14" s="7">
-        <v>43552</v>
+        <v>43625</v>
       </c>
       <c r="D14" s="7">
-        <v>43554</v>
+        <v>43630</v>
       </c>
       <c r="E14" s="10">
-        <f>(C14-DATE(1970,1,1))*86400</f>
-        <v>1553731200</v>
+        <f t="shared" si="0"/>
+        <v>1560038400</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>65</v>
+        <v>56</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>55</v>
       </c>
       <c r="H14" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I14" t="s">
         <v>13</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="7">
+        <v>43641</v>
+      </c>
+      <c r="D15" s="7">
+        <v>43642</v>
+      </c>
+      <c r="E15" s="10">
+        <f t="shared" si="0"/>
+        <v>1561420800</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="7">
-        <v>43625</v>
-      </c>
-      <c r="D15" s="7">
-        <v>43630</v>
-      </c>
-      <c r="E15" s="10">
-        <f>(C15-DATE(1970,1,1))*86400</f>
-        <v>1560038400</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="H15" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
-        <v>14</v>
-      </c>
       <c r="B16" s="9" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="C16" s="7">
-        <v>43641</v>
+        <v>43525</v>
       </c>
       <c r="D16" s="7">
-        <v>43642</v>
+        <v>43525</v>
       </c>
       <c r="E16" s="10">
-        <f>(C16-DATE(1970,1,1))*86400</f>
-        <v>1561420800</v>
+        <f t="shared" si="0"/>
+        <v>1551398400</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="K16" s="9" t="s">
-        <v>24</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="136" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="7">
+        <v>43535</v>
+      </c>
+      <c r="D17" s="7">
+        <v>43535</v>
+      </c>
+      <c r="E17" s="10">
+        <f t="shared" si="0"/>
+        <v>1552262400</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L17">
+  <sortState ref="A2:L16">
     <sortCondition ref="C1"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="G16" r:id="rId1" xr:uid="{1E644AB0-1CE4-CA43-BC4B-C485696BC585}"/>
-    <hyperlink ref="G11" r:id="rId2" xr:uid="{435D4641-689C-4342-BC3A-BE8C2BA92CAC}"/>
-    <hyperlink ref="G15" r:id="rId3" xr:uid="{0EF61B36-07A0-E64B-969C-AA716B3488A5}"/>
+    <hyperlink ref="G15" r:id="rId1" xr:uid="{1E644AB0-1CE4-CA43-BC4B-C485696BC585}"/>
+    <hyperlink ref="G10" r:id="rId2" xr:uid="{435D4641-689C-4342-BC3A-BE8C2BA92CAC}"/>
+    <hyperlink ref="G14" r:id="rId3" xr:uid="{0EF61B36-07A0-E64B-969C-AA716B3488A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Removed old events. Updated new events not on NIH COE
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4F19E2-4732-9844-AB85-A94D1E0EDE11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2250F9-5B58-E345-B778-AE6FE2F43B20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="460" windowWidth="27580" windowHeight="16300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17660" yWindow="11260" windowWidth="27580" windowHeight="16300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
   <si>
     <t>type</t>
   </si>
@@ -69,36 +69,15 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>BIOINFORMATICS-SIG-L listserv</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
     <t>BIOINFO-GENERAL-NCI listserv</t>
   </si>
   <si>
-    <t>Conference</t>
-  </si>
-  <si>
-    <t>The meeting is intended to promote cross-disciplinary exchange between experimental, computational and mathematical biologists studying the organization, functions and regulation of the immune system at various scales. Our goal is to establish a recurrent forum that brings together immunologists and systems biologists in this nascent field.</t>
-  </si>
-  <si>
-    <t>Systems Immunology</t>
-  </si>
-  <si>
-    <t>Cold Spring Harbor, NY</t>
-  </si>
-  <si>
-    <t>https://meetings.cshl.edu/meetings.aspx?meet=SYSIMM&amp;year=19</t>
-  </si>
-  <si>
     <t>Workshop</t>
   </si>
   <si>
-    <t>immunology</t>
-  </si>
-  <si>
     <t>Rockefeller University</t>
   </si>
   <si>
@@ -114,18 +93,6 @@
     <t xml:space="preserve"> To see a list of past workshops, visit http://bioc2018.bioconductor.org.</t>
   </si>
   <si>
-    <t>The course will begin with the workflow involved in moving from platform images to sequence generation, after which participants will gain practical skills for evaluating sequence read quality, mapping reads to a reference genome, and analyzing sequence reads for variation and expression level. The course will conclude with pathway and network analysis on the resultant 'gene' list. Participants will gain experience in cloud computing and data visualization tools. All class exercises will be self-contained units that include example data (e.g., Illumina paired-end data) as well as detailed instructions for installing all required bioinformatics tools.</t>
-  </si>
-  <si>
-    <t>High-Throughput Biology: From Sequence to Networks CSHL Course</t>
-  </si>
-  <si>
-    <t>https://meetings.cshl.edu/courses.aspx?course=C-cbw&amp;year=19</t>
-  </si>
-  <si>
-    <t>1 Bungtown Road Cold Spring Harbor, NY 11724-2213</t>
-  </si>
-  <si>
     <t>Seminar</t>
   </si>
   <si>
@@ -145,51 +112,6 @@
   </si>
   <si>
     <t>Oak Ridge National Laboratory, 8640 Nano Center Drive Oak Ridge, TN 37830</t>
-  </si>
-  <si>
-    <t>Hilton Birmingham at UAB 808 20th Street South, Birmingham, AL 35205</t>
-  </si>
-  <si>
-    <t>http://mcbios19.informatics.uab.edu</t>
-  </si>
-  <si>
-    <t>MCBIOS annual conference is a premier annual meeting for bioinformatics researchers, professionals, and trainees in the Middle and Southern areas of the United States. It is a major venue for informaticians to exchange late-breaking research results, learn technological trends, and network in the region. This annual event is organized by the MCBIOS society (www.mcbios.org) and serves as an affiliate satellite meeting of the International Society of Computational Biology (ISCB, www.iscb.org). MCBIOS 2019 will be hosted by the University of Alabama at Birmingham School of Medicine and co-sponsored by various academic and industrial entities related to genomics, informatics, health sciences, and biopharmaceuticals. We welcome researchers in all career stages (students, postdocs, junior faculty, and experienced researchers) to disseminate late-breaking interdisciplinary research results at this meeting.</t>
-  </si>
-  <si>
-    <t>data integration,RNA biology,genomics,drug discovery,ontology,visualization</t>
-  </si>
-  <si>
-    <t>Informatics for Precision Medicine 16th Annual Conference of the Midsouth Computational Biology &amp; Bioinformatics Society (MCBIOS ’19)</t>
-  </si>
-  <si>
-    <t>A Hole New View: Structure-Function Mapping of the Nuclear Pore Complex</t>
-  </si>
-  <si>
-    <t>NIH Main Campus, Building 35, Room 640</t>
-  </si>
-  <si>
-    <t>mapping</t>
-  </si>
-  <si>
-    <t>NIHLIB-L listserv</t>
-  </si>
-  <si>
-    <t>Electronic Lab Notebook (ELN) Forum</t>
-  </si>
-  <si>
-    <t>NIH Main Campus, Lipsett Amphitheater, Building 10</t>
-  </si>
-  <si>
-    <t>https://www.nihlibrary.nih.gov/electronic-lab-notebook-forum</t>
-  </si>
-  <si>
-    <t>Meeting</t>
-  </si>
-  <si>
-    <t>Presented by the NIH Library, this one-day event will focus on exploring the benefits and challenges of ELN implementation and use. The program will include presentations on a variety of ELN solutions from industry experts, followed by presentations from NIH staff who will address ELN usability, administration, and security. Additional details will be forthcoming as the event draws closer, but be sure to save the date for this exciting event on your 2019 calendars now. For more information, contact Candace Norton (candace.norton@nih.gov).</t>
-  </si>
-  <si>
-    <t>ELN</t>
   </si>
   <si>
     <t>Statistical Methods for Functional Genomics CSHL Course</t>
@@ -221,6 +143,58 @@
 • Predictive modeling of gene regulatory networks using machine learning
 • Analysis of posttranscriptional regulation, RNA binding proteins, and microRNAs
 Format: Detailed lectures and presentations by instructors and guest speakers will be combined with hands-on computer tutorials. The methods covered in the lectures will be applied to example high-throughput data sets.</t>
+  </si>
+  <si>
+    <t>Bioioinformatics User Forum: Single Cell Sequencing</t>
+  </si>
+  <si>
+    <t>NCI Advanced Technology Research Facility, E-1106</t>
+  </si>
+  <si>
+    <t>sequencing, genomics</t>
+  </si>
+  <si>
+    <t>Statistics for Lunch: Survival Analysis</t>
+  </si>
+  <si>
+    <t>NCI Building 549 Auditorium</t>
+  </si>
+  <si>
+    <t>https://abcsfrederick.info/seminars/2019/04/18/BUF.html</t>
+  </si>
+  <si>
+    <t>Come join us for our next Bioinformatics User Forum Meeting where we will be discussing Single Cell Analysis.
+Speakers and Topics:
+Monika Mehta: Single-cell genomics – a glimpse of the current technologies
+Mike Kelly: Single-cell genomics – upcoming technologies
+Vicky Chen: Single Cell Transcriptome Analysis Pipeline</t>
+  </si>
+  <si>
+    <t>Dr George Nelson will be presenting an Introduction to Survival Analysis at our next Statistics for Lunch seminar.
+How do you analyze time-to-event data?
+What is censoring and why is it important?
+What is the difference between a Kaplan Meier estimator and a Cox Proportional Hazards model?</t>
+  </si>
+  <si>
+    <t>https://abcsfrederick.info/seminars/2019/04/25/Stats4Lunch.html</t>
+  </si>
+  <si>
+    <t>BIOINFORMATICS-SIG listserv</t>
+  </si>
+  <si>
+    <t>NLM Reproducibility in Bioinformatics Workshop</t>
+  </si>
+  <si>
+    <t>6001 Executive Boulevard</t>
+  </si>
+  <si>
+    <t>http://bit.ly/repro-workshop-spring-2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The National Library of Medicine is hosting a three-day Reproducibility in Bioinformatics Workshop from May 15 to 17, 2019. Reproducibility can be defined as the ability of a researcher to duplicate the results of a prior study using the same materials and procedures as were used by the original investigator. Reproducibility has become a priority at NIH, requiring that researchers adopt best practices to facilitate replicable research early on. In bioinformatics, that requires adopting computational tools that allow analysis pipelines to be reused and providing sufficient documentation for increased transparency. </t>
+  </si>
+  <si>
+    <t>tools, reproducibility</t>
   </si>
 </sst>
 </file>
@@ -256,7 +230,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF24292E"/>
+      <color rgb="FF212529"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -304,7 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -322,23 +296,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -620,19 +583,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.1640625" customWidth="1"/>
     <col min="2" max="2" width="55.6640625" style="7" customWidth="1"/>
-    <col min="3" max="4" width="10.83203125" style="14"/>
-    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" style="11"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="89.1640625" style="7" customWidth="1"/>
     <col min="7" max="7" width="70.83203125" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="104.33203125" style="3" customWidth="1"/>
@@ -647,10 +610,10 @@
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -678,296 +641,224 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="8" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="15">
-        <v>43535</v>
-      </c>
-      <c r="D2" s="15">
-        <v>43535</v>
-      </c>
-      <c r="E2" s="16">
-        <f>(C2-DATE(1970,1,1))*86400</f>
-        <v>1552262400</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" s="16" t="s">
+    <row r="2" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="11">
+        <v>43625</v>
+      </c>
+      <c r="D2" s="11">
+        <v>43630</v>
+      </c>
+      <c r="E2" s="8">
+        <f t="shared" ref="E2:E4" si="0">(C2-DATE(1970,1,1))*86400</f>
+        <v>1560038400</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="11"/>
+      <c r="B3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="11">
+        <v>43641</v>
+      </c>
+      <c r="D3" s="11">
+        <v>43642</v>
+      </c>
+      <c r="E3" s="8">
+        <f t="shared" si="0"/>
+        <v>1561420800</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" ht="102" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="14">
-        <v>43535</v>
-      </c>
-      <c r="D3" s="14">
-        <v>43541</v>
-      </c>
-      <c r="E3" s="8">
-        <f t="shared" ref="E3:E9" si="0">(C3-DATE(1970,1,1))*86400</f>
-        <v>1552262400</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" t="s">
+    <row r="4" spans="1:12" ht="404" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="B4" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="15">
-        <v>43537</v>
-      </c>
-      <c r="D4" s="15">
-        <v>43540</v>
+      <c r="C4" s="11">
+        <v>43644</v>
+      </c>
+      <c r="D4" s="11">
+        <v>43657</v>
       </c>
       <c r="E4" s="8">
         <f t="shared" si="0"/>
-        <v>1552435200</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>18</v>
+        <v>1561680000</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="11"/>
-    </row>
-    <row r="5" spans="1:12" ht="136" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
-        <v>14</v>
-      </c>
       <c r="B5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="14">
-        <v>43552</v>
-      </c>
-      <c r="D5" s="14">
-        <v>43554</v>
-      </c>
-      <c r="E5" s="8">
-        <f t="shared" si="0"/>
-        <v>1553731200</v>
+        <v>32</v>
+      </c>
+      <c r="C5" s="11">
+        <v>43573</v>
+      </c>
+      <c r="D5" s="11">
+        <v>43573</v>
+      </c>
+      <c r="E5">
+        <v>1555588800</v>
       </c>
       <c r="F5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="K5" s="7" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="14">
-        <v>43625</v>
-      </c>
-      <c r="D6" s="14">
-        <v>43630</v>
-      </c>
-      <c r="E6" s="8">
-        <f t="shared" si="0"/>
-        <v>1560038400</v>
+        <v>35</v>
+      </c>
+      <c r="C6" s="11">
+        <v>43580</v>
+      </c>
+      <c r="D6" s="11">
+        <v>43580</v>
+      </c>
+      <c r="E6" s="12">
+        <v>1556191800</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="H6" t="s">
+      <c r="G6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I6" t="s">
-        <v>13</v>
+      <c r="I6" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="11">
+        <v>43600</v>
+      </c>
+      <c r="D7" s="11">
+        <v>43602</v>
+      </c>
+      <c r="E7">
+        <v>1557910800</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="14">
-        <v>43641</v>
-      </c>
-      <c r="D7" s="14">
-        <v>43642</v>
-      </c>
-      <c r="E7" s="8">
-        <f t="shared" si="0"/>
-        <v>1561420800</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="I7" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="14">
-        <v>43525</v>
-      </c>
-      <c r="D8" s="14">
-        <v>43525</v>
-      </c>
-      <c r="E8" s="8">
-        <f t="shared" si="0"/>
-        <v>1551398400</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="404" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="14">
-        <v>43644</v>
-      </c>
-      <c r="D9" s="14">
-        <v>43657</v>
-      </c>
-      <c r="E9" s="8">
-        <f t="shared" si="0"/>
-        <v>1561680000</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L8">
+  <sortState ref="A2:L3">
     <sortCondition ref="C1"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="G7" r:id="rId1" xr:uid="{1E644AB0-1CE4-CA43-BC4B-C485696BC585}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{435D4641-689C-4342-BC3A-BE8C2BA92CAC}"/>
-    <hyperlink ref="G6" r:id="rId3" xr:uid="{0EF61B36-07A0-E64B-969C-AA716B3488A5}"/>
-    <hyperlink ref="G9" r:id="rId4" xr:uid="{9529D7C5-7F55-B84C-B674-5FB258E9822A}"/>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{1E644AB0-1CE4-CA43-BC4B-C485696BC585}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{0EF61B36-07A0-E64B-969C-AA716B3488A5}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{9529D7C5-7F55-B84C-B674-5FB258E9822A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Updated with new events, including BCBB seminars
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2250F9-5B58-E345-B778-AE6FE2F43B20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26333DC1-197B-8D47-87CA-E55AE29039C4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17660" yWindow="11260" windowWidth="27580" windowHeight="16300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22240" yWindow="460" windowWidth="27580" windowHeight="16300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,16 @@
   <definedNames>
     <definedName name="_Hlk518048214" localSheetId="0">events!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="75">
   <si>
     <t>type</t>
   </si>
@@ -145,29 +151,10 @@
 Format: Detailed lectures and presentations by instructors and guest speakers will be combined with hands-on computer tutorials. The methods covered in the lectures will be applied to example high-throughput data sets.</t>
   </si>
   <si>
-    <t>Bioioinformatics User Forum: Single Cell Sequencing</t>
-  </si>
-  <si>
-    <t>NCI Advanced Technology Research Facility, E-1106</t>
-  </si>
-  <si>
-    <t>sequencing, genomics</t>
-  </si>
-  <si>
     <t>Statistics for Lunch: Survival Analysis</t>
   </si>
   <si>
     <t>NCI Building 549 Auditorium</t>
-  </si>
-  <si>
-    <t>https://abcsfrederick.info/seminars/2019/04/18/BUF.html</t>
-  </si>
-  <si>
-    <t>Come join us for our next Bioinformatics User Forum Meeting where we will be discussing Single Cell Analysis.
-Speakers and Topics:
-Monika Mehta: Single-cell genomics – a glimpse of the current technologies
-Mike Kelly: Single-cell genomics – upcoming technologies
-Vicky Chen: Single Cell Transcriptome Analysis Pipeline</t>
   </si>
   <si>
     <t>Dr George Nelson will be presenting an Introduction to Survival Analysis at our next Statistics for Lunch seminar.
@@ -195,6 +182,116 @@
   </si>
   <si>
     <t>tools, reproducibility</t>
+  </si>
+  <si>
+    <t>Overview of Statistics: Statistical Testing</t>
+  </si>
+  <si>
+    <t>NIAID BioIT listserv</t>
+  </si>
+  <si>
+    <t>NIH Main Campus, Building 10, Room 11S235 (Wolff Conference Room)</t>
+  </si>
+  <si>
+    <t>https://events.eventzilla.net/e/overview-of-statistics-statistical-testing-2138748916</t>
+  </si>
+  <si>
+    <t>Description:
+A statistical test provides a mechanism for making quantitative decisions about a process or processes. Its intent is to determine whether there is enough evidence to reject a null hypothesis or hypothesis about the process. This course will cover designing the statistical testing process, data preprocessing, understanding and interpreting the basic statistical concepts (p-value, confidence interval, etc.), and the most common statistical testing methods in clinical research. The course will also include a hands-on component using GraphPad Prism and R statistical language to perform common statistical tests. 
+Topics that will be covered in this course include: 
+- Introduction to the statistical testing process 
+- Data preprocessing 
+- Common parametric and non-parametric tests including two-sample t-test, ANOVA, multiple comparisons, correlation, linear regression, robust statistics, etc. 
+- Application in GraphPad Prism and R</t>
+  </si>
+  <si>
+    <t>biostatistics,testing</t>
+  </si>
+  <si>
+    <t>Introduction to Categorical Data Analysis</t>
+  </si>
+  <si>
+    <t>NIH Main Campus, Building 40</t>
+  </si>
+  <si>
+    <t>https://events.eventzilla.net/e/introduction-to-categorical-data-analysis-2138747015</t>
+  </si>
+  <si>
+    <t>Description:
+Categorical data is the data type consisting of categorical variables or of data converted into categories or groups. Categorical data analysis is vital and useful statistical analysis in clinical research since categorical data occupies a large portion of the data we collect and use. This course will start by introducing different types of categorical data and characteristics, contingency tables, and probability distribution to learn how to calculate and interpret some useful statistics such as odds ratio and relative risk. The last section will cover different types of statistical testing for categorical data by cases. Each example will include a hands-on component using R Studio to perform the analysis. 
+Topics that will be covered in this course include: 
+- Analyzing contingency tables (positive/negative predictive value, sensitivity, specificity, Type I/II error, joint, marginal, conditional association)
+- Measuring the strength of association (odds ratio, relative risk)
+- Statistical testing of independence (cases with nominal large sample size data and small sample size data, cases with stratified and paired data, cases with ordinal data)</t>
+  </si>
+  <si>
+    <t>biostatistics,data analysis</t>
+  </si>
+  <si>
+    <t>Introduction to Exome Sequencing and Variant Analysis</t>
+  </si>
+  <si>
+    <t>NIH Main Campus, Building 50, Room 6334</t>
+  </si>
+  <si>
+    <t>https://events.eventzilla.net/e/introduction-to-exome-sequencing-and-variant-analysis-2138748918</t>
+  </si>
+  <si>
+    <t>Attendees will learn how to use GATK, Picard, and other tools to do QC, variant calling, annotation, and candidate variant selection for whole exome sequencing data on the NIAID HPC (LOCUS).</t>
+  </si>
+  <si>
+    <t>exome,variant analysis</t>
+  </si>
+  <si>
+    <t>Virus Sequence Alignment and Phylogenetics</t>
+  </si>
+  <si>
+    <t>https://events.eventzilla.net/e/virus-sequence-alignment-and-phylogenetics-2138748919</t>
+  </si>
+  <si>
+    <t>Virus sequence data are exceptionally interesting for molecular evolutionary analysis due to their typically rapid accumulation of SNPs and large population sizes. In this lecture, we will review the basis for DNA sequence alignment and phylogenetics and the major algorithms used to construct phylogenetic trees. We will perform an example multiple sequence alignment and phylogenetic analyses using two of these algorithms.</t>
+  </si>
+  <si>
+    <t>phylogenetics,DNA sequence alignment</t>
+  </si>
+  <si>
+    <t>MICROBIOME listserv</t>
+  </si>
+  <si>
+    <t>3rd NIH-FDA Joint Microbiome Working Group</t>
+  </si>
+  <si>
+    <t>NIH Main Campus, Building 10, Lipsett Auditorium</t>
+  </si>
+  <si>
+    <t>https://ncifrederick.cancer.gov/events/conferences/3rd-nih-fda-joint-microbiome-working-group</t>
+  </si>
+  <si>
+    <t>Working Group</t>
+  </si>
+  <si>
+    <t>This meeting brings together staff from across the intramural NIH and FDA laboratories. Its major purpose is to foster communication, cooperation, and collaborations across NIH institutes and the FDA regarding ongoing microbiome research.</t>
+  </si>
+  <si>
+    <t>microbiome</t>
+  </si>
+  <si>
+    <t>https://www.signupgenius.com/go/60B0B44A9A82BA5FD0-nvidia</t>
+  </si>
+  <si>
+    <t>NVIDIA Consultations</t>
+  </si>
+  <si>
+    <t>NIH, Ft. Detrick</t>
+  </si>
+  <si>
+    <t>Consultation</t>
+  </si>
+  <si>
+    <t>NVIDIA will be coming to Ft Detrick on May 8 to provide one-on-one consultations for your deep learning needs. The expectation for this consultation is that you show up with questions. They will be able to answer questions ranging from what studies might be reasonable for you to plan, to how to get your feet wet with your first deep learning model, up through fine tuning a model on your local GPU or on Biowulf.</t>
+  </si>
+  <si>
+    <t>deep learning</t>
   </si>
 </sst>
 </file>
@@ -204,7 +301,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/m/dd"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -224,13 +321,6 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF212529"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -301,7 +391,7 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -583,11 +673,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,7 +745,7 @@
         <v>43630</v>
       </c>
       <c r="E2" s="8">
-        <f t="shared" ref="E2:E4" si="0">(C2-DATE(1970,1,1))*86400</f>
+        <f t="shared" ref="E2:E40" si="0">(C2-DATE(1970,1,1))*86400</f>
         <v>1560038400</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -749,7 +839,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>13</v>
       </c>
@@ -757,19 +847,20 @@
         <v>32</v>
       </c>
       <c r="C5" s="11">
-        <v>43573</v>
+        <v>43580</v>
       </c>
       <c r="D5" s="11">
-        <v>43573</v>
-      </c>
-      <c r="E5">
-        <v>1555588800</v>
+        <v>43580</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" si="0"/>
+        <v>1556150400</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>33</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>20</v>
@@ -778,87 +869,270 @@
         <v>12</v>
       </c>
       <c r="J5" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="11">
+        <v>43600</v>
+      </c>
+      <c r="D6" s="11">
+        <v>43602</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" si="0"/>
+        <v>1557878400</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="85" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="11">
-        <v>43580</v>
-      </c>
-      <c r="D6" s="11">
-        <v>43580</v>
-      </c>
-      <c r="E6" s="12">
-        <v>1556191800</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>36</v>
-      </c>
       <c r="G6" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>12</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="238" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>42</v>
       </c>
       <c r="C7" s="11">
-        <v>43600</v>
+        <v>43585</v>
       </c>
       <c r="D7" s="11">
-        <v>43602</v>
-      </c>
-      <c r="E7">
-        <v>1557910800</v>
+        <v>43585</v>
+      </c>
+      <c r="E7" s="8">
+        <f t="shared" si="0"/>
+        <v>1556582400</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>12</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="11">
+        <v>43605</v>
+      </c>
+      <c r="D8" s="11">
+        <v>43605</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="0"/>
+        <v>1558310400</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="11">
+        <v>43629</v>
+      </c>
+      <c r="D9" s="11">
+        <v>43629</v>
+      </c>
+      <c r="E9" s="8">
+        <f t="shared" si="0"/>
+        <v>1560384000</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="11">
+        <v>43637</v>
+      </c>
+      <c r="D10" s="11">
+        <v>43637</v>
+      </c>
+      <c r="E10" s="8">
+        <f t="shared" si="0"/>
+        <v>1561075200</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="11">
+        <v>43619</v>
+      </c>
+      <c r="D11" s="11">
+        <v>43619</v>
+      </c>
+      <c r="E11" s="8">
+        <f t="shared" si="0"/>
+        <v>1559520000</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="11">
+        <v>43593</v>
+      </c>
+      <c r="D12" s="11">
+        <v>43593</v>
+      </c>
+      <c r="E12" s="8">
+        <f t="shared" si="0"/>
+        <v>1557273600</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L3">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L3">
     <sortCondition ref="C1"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" xr:uid="{1E644AB0-1CE4-CA43-BC4B-C485696BC585}"/>
     <hyperlink ref="G2" r:id="rId2" xr:uid="{0EF61B36-07A0-E64B-969C-AA716B3488A5}"/>
     <hyperlink ref="G4" r:id="rId3" xr:uid="{9529D7C5-7F55-B84C-B674-5FB258E9822A}"/>
+    <hyperlink ref="G12" r:id="rId4" tooltip="https://www.signupgenius.com/go/60B0B44A9A82BA5FD0-nvidia" xr:uid="{5267E26C-5180-BB4E-BDDB-60A73296D1DC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Updated 5/2 with new events
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26333DC1-197B-8D47-87CA-E55AE29039C4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8D4D23-0FA8-6248-9549-8854E84D5CC5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22240" yWindow="460" windowWidth="27580" windowHeight="16300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24120" yWindow="460" windowWidth="27580" windowHeight="16300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -151,21 +151,6 @@
 Format: Detailed lectures and presentations by instructors and guest speakers will be combined with hands-on computer tutorials. The methods covered in the lectures will be applied to example high-throughput data sets.</t>
   </si>
   <si>
-    <t>Statistics for Lunch: Survival Analysis</t>
-  </si>
-  <si>
-    <t>NCI Building 549 Auditorium</t>
-  </si>
-  <si>
-    <t>Dr George Nelson will be presenting an Introduction to Survival Analysis at our next Statistics for Lunch seminar.
-How do you analyze time-to-event data?
-What is censoring and why is it important?
-What is the difference between a Kaplan Meier estimator and a Cox Proportional Hazards model?</t>
-  </si>
-  <si>
-    <t>https://abcsfrederick.info/seminars/2019/04/25/Stats4Lunch.html</t>
-  </si>
-  <si>
     <t>BIOINFORMATICS-SIG listserv</t>
   </si>
   <si>
@@ -184,28 +169,7 @@
     <t>tools, reproducibility</t>
   </si>
   <si>
-    <t>Overview of Statistics: Statistical Testing</t>
-  </si>
-  <si>
     <t>NIAID BioIT listserv</t>
-  </si>
-  <si>
-    <t>NIH Main Campus, Building 10, Room 11S235 (Wolff Conference Room)</t>
-  </si>
-  <si>
-    <t>https://events.eventzilla.net/e/overview-of-statistics-statistical-testing-2138748916</t>
-  </si>
-  <si>
-    <t>Description:
-A statistical test provides a mechanism for making quantitative decisions about a process or processes. Its intent is to determine whether there is enough evidence to reject a null hypothesis or hypothesis about the process. This course will cover designing the statistical testing process, data preprocessing, understanding and interpreting the basic statistical concepts (p-value, confidence interval, etc.), and the most common statistical testing methods in clinical research. The course will also include a hands-on component using GraphPad Prism and R statistical language to perform common statistical tests. 
-Topics that will be covered in this course include: 
-- Introduction to the statistical testing process 
-- Data preprocessing 
-- Common parametric and non-parametric tests including two-sample t-test, ANOVA, multiple comparisons, correlation, linear regression, robust statistics, etc. 
-- Application in GraphPad Prism and R</t>
-  </si>
-  <si>
-    <t>biostatistics,testing</t>
   </si>
   <si>
     <t>Introduction to Categorical Data Analysis</t>
@@ -292,6 +256,33 @@
   </si>
   <si>
     <t>deep learning</t>
+  </si>
+  <si>
+    <t>Reproducible workflows with Snakemake</t>
+  </si>
+  <si>
+    <t>NIH Main Campus, Building 10, FAES classrooms 1 &amp; 2</t>
+  </si>
+  <si>
+    <t>The workshop has limited seats. Please indicate your interest by emailing ryan.dale@nih.gov.</t>
+  </si>
+  <si>
+    <t>workflow</t>
+  </si>
+  <si>
+    <t>ChIP-Seq Data Analysis: Probing DNA-Protein Interactions</t>
+  </si>
+  <si>
+    <t>NIH Bldg 37, Rm 2041/2107</t>
+  </si>
+  <si>
+    <t>https://btep.ccr.cancer.gov/classes/chip/</t>
+  </si>
+  <si>
+    <t>This workshop will teach the basic concepts and practical aspects of data analysis. Topics covered will include: experimental approach, quality control, peak calling, and basic biological interpretation. No computer is required for this class, there is no hands-on work.</t>
+  </si>
+  <si>
+    <t>data analysis,ChIP-Seq,quality control,peak calling,interpretation</t>
   </si>
 </sst>
 </file>
@@ -675,9 +666,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -745,7 +736,7 @@
         <v>43630</v>
       </c>
       <c r="E2" s="8">
-        <f t="shared" ref="E2:E40" si="0">(C2-DATE(1970,1,1))*86400</f>
+        <f t="shared" ref="E2:E12" si="0">(C2-DATE(1970,1,1))*86400</f>
         <v>1560038400</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -839,97 +830,100 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" s="11">
-        <v>43580</v>
+        <v>43600</v>
       </c>
       <c r="D5" s="11">
-        <v>43580</v>
+        <v>43602</v>
       </c>
       <c r="E5" s="8">
         <f t="shared" si="0"/>
-        <v>1556150400</v>
+        <v>1557878400</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>12</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="238" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C6" s="11">
-        <v>43600</v>
+        <v>43605</v>
       </c>
       <c r="D6" s="11">
-        <v>43602</v>
+        <v>43605</v>
       </c>
       <c r="E6" s="8">
         <f t="shared" si="0"/>
-        <v>1557878400</v>
+        <v>1558310400</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>12</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C7" s="11">
-        <v>43585</v>
+        <v>43629</v>
       </c>
       <c r="D7" s="11">
-        <v>43585</v>
+        <v>43629</v>
       </c>
       <c r="E7" s="8">
         <f t="shared" si="0"/>
-        <v>1556582400</v>
+        <v>1560384000</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>20</v>
@@ -938,31 +932,31 @@
         <v>12</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C8" s="11">
-        <v>43605</v>
+        <v>43637</v>
       </c>
       <c r="D8" s="11">
-        <v>43605</v>
+        <v>43637</v>
       </c>
       <c r="E8" s="8">
         <f t="shared" si="0"/>
-        <v>1558310400</v>
+        <v>1561075200</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>50</v>
@@ -980,115 +974,112 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C9" s="11">
-        <v>43629</v>
+        <v>43619</v>
       </c>
       <c r="D9" s="11">
-        <v>43629</v>
+        <v>43619</v>
       </c>
       <c r="E9" s="8">
         <f t="shared" si="0"/>
-        <v>1560384000</v>
+        <v>1559520000</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>12</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C10" s="11">
-        <v>43637</v>
+        <v>43593</v>
       </c>
       <c r="D10" s="11">
-        <v>43637</v>
+        <v>43593</v>
       </c>
       <c r="E10" s="8">
         <f t="shared" si="0"/>
-        <v>1561075200</v>
+        <v>1557273600</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>59</v>
+        <v>62</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>12</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C11" s="11">
-        <v>43619</v>
+        <v>43605</v>
       </c>
       <c r="D11" s="11">
-        <v>43619</v>
+        <v>43605</v>
       </c>
       <c r="E11" s="8">
         <f t="shared" si="0"/>
-        <v>1559520000</v>
+        <v>1558310400</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>12</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
@@ -1096,23 +1087,23 @@
         <v>70</v>
       </c>
       <c r="C12" s="11">
-        <v>43593</v>
+        <v>43595</v>
       </c>
       <c r="D12" s="11">
-        <v>43593</v>
+        <v>43595</v>
       </c>
       <c r="E12" s="8">
         <f t="shared" si="0"/>
-        <v>1557273600</v>
+        <v>1557446400</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G12" s="12" t="s">
-        <v>69</v>
+      <c r="G12" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>12</v>
@@ -1132,7 +1123,7 @@
     <hyperlink ref="G3" r:id="rId1" xr:uid="{1E644AB0-1CE4-CA43-BC4B-C485696BC585}"/>
     <hyperlink ref="G2" r:id="rId2" xr:uid="{0EF61B36-07A0-E64B-969C-AA716B3488A5}"/>
     <hyperlink ref="G4" r:id="rId3" xr:uid="{9529D7C5-7F55-B84C-B674-5FB258E9822A}"/>
-    <hyperlink ref="G12" r:id="rId4" tooltip="https://www.signupgenius.com/go/60B0B44A9A82BA5FD0-nvidia" xr:uid="{5267E26C-5180-BB4E-BDDB-60A73296D1DC}"/>
+    <hyperlink ref="G10" r:id="rId4" tooltip="https://www.signupgenius.com/go/60B0B44A9A82BA5FD0-nvidia" xr:uid="{5267E26C-5180-BB4E-BDDB-60A73296D1DC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
updated with new microbiome conference
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F11BC07-C432-D84C-A281-1DDF36BEA691}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8183A3-13B3-124A-AF50-00B38FF0D998}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,30 +75,28 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>https://gen.omeclk.com/portal/deployforward/Forward.jsp?mEAM7shKWZU0TQsD9kmKCKMgCAYm%2BVauA</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Seminar</t>
-  </si>
-  <si>
-    <t>Advances in our understanding of the microbiome represent one of the most exciting fields of modern biomedical research. Our microbiomes change every day through the foods we eat, the environments we experience, even the people we live and work with. The implications of microbiome changes for our health are just beginning to be understood.
-Through the American Gut Project—the largest crowdsourced and crowdfunded citizen-science project yet conducted—we now know about the microbiomes of many types of people, from the healthiest athletes and centenarians to the sickest cancer and intensive-care patients. Diet has an especially profound effect on our microbiomes, often outweighing the effects of disease or medications. This raises the prospect of a system for real-time microbiome analysis that helps guide our daily decisions in a way that optimizes our microbiomes for life-long wellness.
-A live Q&amp;A session will follow the presentation, offering you a chance to pose questions to our expert keynote speaker.</t>
-  </si>
-  <si>
     <t>microbiome,analysis</t>
   </si>
   <si>
     <t>MICROBIOME listserv</t>
   </si>
   <si>
-    <t>THE DYNAMIC MICROBIOME</t>
-  </si>
-  <si>
-    <t>Online</t>
+    <t>6th Annual Translational Microbiome Conference</t>
+  </si>
+  <si>
+    <t>The Westin Copley Place 10 Huntington Avenue Boston, MA 02116 USA</t>
+  </si>
+  <si>
+    <t>https://microbiomeconference.com</t>
+  </si>
+  <si>
+    <t>Conference</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>The conference will bring together the leading microbiome companies working to successfully commercialize microbiome-based diagnostics, therapeutics, adjunct therapies and direct-to-consumer services and products across a range of therapeutic areas, from gut to skin and beyond. Expanding on this core focus year on year, the conference continues to offer informative, hands-on workshops, panels sponsored and directed by industry to focus on your concerns and tightly curated content that goes beyond the usual infomercials to provide tangible and useful insights to how your peers are addressing their commercial approach to the space.</t>
   </si>
 </sst>
 </file>
@@ -166,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -186,7 +184,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,11 +464,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,39 +522,39 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="10">
+        <v>43942</v>
+      </c>
+      <c r="D2" s="10">
+        <v>43944</v>
+      </c>
+      <c r="E2" s="8">
+        <v>1587499573</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="10">
-        <v>43816</v>
-      </c>
-      <c r="D2" s="10">
-        <v>43816</v>
-      </c>
-      <c r="E2" s="11">
-        <v>1576540800</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="J2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -572,9 +569,6 @@
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E7" s="8"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Updated with new microbiome event
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8183A3-13B3-124A-AF50-00B38FF0D998}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61339B27-04A5-2A4B-BE47-1132D2688FB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>type</t>
   </si>
@@ -97,6 +97,27 @@
   </si>
   <si>
     <t>The conference will bring together the leading microbiome companies working to successfully commercialize microbiome-based diagnostics, therapeutics, adjunct therapies and direct-to-consumer services and products across a range of therapeutic areas, from gut to skin and beyond. Expanding on this core focus year on year, the conference continues to offer informative, hands-on workshops, panels sponsored and directed by industry to focus on your concerns and tightly curated content that goes beyond the usual infomercials to provide tangible and useful insights to how your peers are addressing their commercial approach to the space.</t>
+  </si>
+  <si>
+    <t>Malibu Microbiome Meeting</t>
+  </si>
+  <si>
+    <t>Villa Graziadio Executive Center at Pepperdine University 24255 Pacific Coast Hwy Malibu, CA 90263</t>
+  </si>
+  <si>
+    <t>https://malibumicrobiomemeeting.com/home</t>
+  </si>
+  <si>
+    <t>Program highlights include:
+Understanding Microbiome Standards and Research
+Nutrition and the Microbiome
+Update on C. difficile
+Other applications of FMT
+Manufactured microbial based therapies
+Regulating the human gut microbiome</t>
+  </si>
+  <si>
+    <t>microbiome,analysis,standards</t>
   </si>
 </sst>
 </file>
@@ -468,7 +489,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,8 +578,40 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E3" s="8"/>
+    <row r="3" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="10">
+        <v>43918</v>
+      </c>
+      <c r="D3" s="10">
+        <v>43919</v>
+      </c>
+      <c r="E3" s="8">
+        <v>1583226000</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E4" s="8"/>

</xml_diff>

<commit_message>
Added events for NIAID Bioinformatics Education Support initiative
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61339B27-04A5-2A4B-BE47-1132D2688FB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0011BA77-C212-0044-BA55-1C8576E61FF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7580" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
   <si>
     <t>type</t>
   </si>
@@ -118,6 +118,121 @@
   </si>
   <si>
     <t>microbiome,analysis,standards</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>NIAID BioIT listserv</t>
+  </si>
+  <si>
+    <t>https://attendee.gotowebinar.com/register/3821903923336399627</t>
+  </si>
+  <si>
+    <t>Publishing to NCBI SRA the Easy Way Using METAGENOTE</t>
+  </si>
+  <si>
+    <t>GoToWebinar</t>
+  </si>
+  <si>
+    <t>Seminar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METAGENOTE is a web platform designed at NIAID with the goal of facilitating annotation of samples and associated sequencing data.   Attendees will learn how to use METAGENOTE to add relevant metadata to samples and proceed to publish metadata and sequencing files to NCBI SRA.  The simple submission process automatically creates a BioProject, BioSample entries and the SRA experiment records at NCBI. </t>
+  </si>
+  <si>
+    <t>SRA,sequencing,annotation,genomics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customizing Your Graphs using GraphPad Prism 8 </t>
+  </si>
+  <si>
+    <t>This seminar will cover topics including a basic introduction to GraphPad Prism, how to import data, how to choose and customize graphs for your analysis, and how to export graphs in GraphPad Prism. The seminar is intended for researchers with little to no experience using Prism 8, but almost everyone who uses Prism for visualization could benefit from this event</t>
+  </si>
+  <si>
+    <t>statistics,Prism,visualization</t>
+  </si>
+  <si>
+    <t>https://attendee.gotowebinar.com/register/1445707563108471309</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This seminar will focus on how to choose an appropriate statistical test given data and hypothesis. Specific topics include the following: unpaired t-test, paired t-test, ordinary one-way ANOVA, repeated measures one-way ANOVA and non-parametric tests, Chi-square test and Fisher’s exact test. </t>
+  </si>
+  <si>
+    <t>statistics,tests</t>
+  </si>
+  <si>
+    <t>Practical Training on GraphPad Prism for Statistical Testing - Part I</t>
+  </si>
+  <si>
+    <t>https://attendee.gotowebinar.com/register/324234290079452429</t>
+  </si>
+  <si>
+    <t>https://attendee.gotowebinar.com/register/2693467443169443085</t>
+  </si>
+  <si>
+    <t>Practical Training on GraphPad Prism for Statistical Testing - Part II</t>
+  </si>
+  <si>
+    <t>Introduction to UNIX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The raw output of biological research is usually in the form of large text files. UNIX is particularly suited to working with such files and has several powerful and flexible commands that can process such data. In UNIX user types everything and it may seem archaic to use a keyboard to issue commands today. However, it’s much easier to automate keyboard tasks than mouse tasks and this course is a gentle introduction on UNIX commands can be combined and automated to handle biological data.
+The first part of the course will focus on the file management and parsing of text files in UNIX environment. Second part of the course will focus on simple scripting to manipulate. The course is designed for beginners and will consist hands on exercises along with the lectures. At the end of the course participants will learn basic UNIX commands and will appreciate the real strength of UNIX on how commands can be combined in an almost unlimited fashion. </t>
+  </si>
+  <si>
+    <t>UNIX,file management,scripting</t>
+  </si>
+  <si>
+    <t>https://attendee.gotowebinar.com/register/7767092381286077453</t>
+  </si>
+  <si>
+    <t>Finding Master Genes Through Gene Regulatory Network Analysis</t>
+  </si>
+  <si>
+    <t>One major challenge of a high throughput gene expression study is to accurately spot promising master genes, for costly validation in the wet lab. Fortunately, these master genes and related regulatory networks can be recovered by examining the statistical relationships of gene expression and inferring from known knowledge. In this webinar, we will review the best available approaches and tools to find master genes from the crowd.</t>
+  </si>
+  <si>
+    <t>networks,gene expression</t>
+  </si>
+  <si>
+    <t>https://attendee.gotowebinar.com/register/6504368147971482893</t>
+  </si>
+  <si>
+    <t>Studying the Microbiome Using the Nephele Web Platform</t>
+  </si>
+  <si>
+    <t>This webinar will demonstrate how to process and analyze a 16S microbiome dataset as well as a shotgun metagenomics dataset using the pipelines available in the Nephele platform.</t>
+  </si>
+  <si>
+    <t>microbiome,16S,metagenomics</t>
+  </si>
+  <si>
+    <t>https://attendee.gotowebinar.com/register/4895163611488872973</t>
+  </si>
+  <si>
+    <t>Molecular Visualization with Chimera</t>
+  </si>
+  <si>
+    <t>Hands on demonstration of how to visualize and interrogate a molecular structure using Chimera.  Topics covered will include making selections and changing representations, measuring distances, mapping properties to surfaces, and generating figures for publication.  Chimera software is available from https://www.cgl.ucsf.edu/chimera/download.html</t>
+  </si>
+  <si>
+    <t>Chimera,structure</t>
+  </si>
+  <si>
+    <t>https://attendee.gotowebinar.com/register/4222276788941181965</t>
+  </si>
+  <si>
+    <t>Preparing and Submitting Protein Structures to the NIAID 3D Printing Service</t>
+  </si>
+  <si>
+    <t>This webinar will demonstrate the procedures for creating protein structure visualizations using UCSF Chimera, and the considerations for efficiently submitting them to the NIAID 3D printing service provided by the Bioinformatics and Computational Biosciences Branch (BCBB).  Use of the NIH 3D Print Exchange to generate models will also be discussed: https://3dprint.nih.gov. Note that 3D printing is a free service provided to NIAID to further the mission of the Institute.  Chimera software is available from https://www.cgl.ucsf.edu/chimera/download.html.</t>
+  </si>
+  <si>
+    <t>Chimera,3D print,models</t>
+  </si>
+  <si>
+    <t>https://attendee.gotowebinar.com/register/2509636795587133709</t>
   </si>
 </sst>
 </file>
@@ -485,11 +600,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -569,7 +684,7 @@
         <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>19</v>
@@ -586,13 +701,13 @@
         <v>20</v>
       </c>
       <c r="C3" s="10">
-        <v>43918</v>
+        <v>44065</v>
       </c>
       <c r="D3" s="10">
-        <v>43919</v>
+        <v>44066</v>
       </c>
       <c r="E3" s="8">
-        <v>1583226000</v>
+        <v>1598097600</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>21</v>
@@ -613,14 +728,320 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E6" s="8"/>
+    <row r="4" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="10">
+        <v>43914</v>
+      </c>
+      <c r="D4" s="10">
+        <v>43914</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1585054800</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="10">
+        <v>43915</v>
+      </c>
+      <c r="D5" s="10">
+        <v>43915</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1585130400</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="10">
+        <v>43916</v>
+      </c>
+      <c r="D6" s="10">
+        <v>43916</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1585216800</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="10">
+        <v>43923</v>
+      </c>
+      <c r="D7" s="10">
+        <v>43923</v>
+      </c>
+      <c r="E7">
+        <v>1585821600</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="10">
+        <v>43917</v>
+      </c>
+      <c r="D8" s="10">
+        <v>43917</v>
+      </c>
+      <c r="E8">
+        <v>1585303200</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="10">
+        <v>43920</v>
+      </c>
+      <c r="D9" s="10">
+        <v>43920</v>
+      </c>
+      <c r="E9">
+        <v>1585562400</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="10">
+        <v>43921</v>
+      </c>
+      <c r="D10" s="10">
+        <v>43921</v>
+      </c>
+      <c r="E10">
+        <v>1585659600</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="10">
+        <v>43922</v>
+      </c>
+      <c r="D11" s="10">
+        <v>43922</v>
+      </c>
+      <c r="E11">
+        <v>1585735200</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="10">
+        <v>43923</v>
+      </c>
+      <c r="D12" s="10">
+        <v>43923</v>
+      </c>
+      <c r="E12">
+        <v>1585832400</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added additional seminars to GoToWebinar
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0011BA77-C212-0044-BA55-1C8576E61FF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D106E84-0D09-FC43-B5CA-94914B5F1933}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7580" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="71">
   <si>
     <t>type</t>
   </si>
@@ -135,9 +135,6 @@
     <t>GoToWebinar</t>
   </si>
   <si>
-    <t>Seminar</t>
-  </si>
-  <si>
     <t xml:space="preserve">METAGENOTE is a web platform designed at NIAID with the goal of facilitating annotation of samples and associated sequencing data.   Attendees will learn how to use METAGENOTE to add relevant metadata to samples and proceed to publish metadata and sequencing files to NCBI SRA.  The simple submission process automatically creates a BioProject, BioSample entries and the SRA experiment records at NCBI. </t>
   </si>
   <si>
@@ -233,6 +230,33 @@
   </si>
   <si>
     <t>https://attendee.gotowebinar.com/register/2509636795587133709</t>
+  </si>
+  <si>
+    <t>Webinar</t>
+  </si>
+  <si>
+    <t>Introduction to Geneious for Genomics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This workshop will cover introductory topics for using Geneious including basic navigation, plugins, and import/export of files (including from other software, like Vector NTI).  We will also go through some examples of Primer Design, Cloning, and CRISPR site-finding, while also learning how to search NCBI and other databases and create automated workflows. </t>
+  </si>
+  <si>
+    <t>genomics,Geneious,primer design</t>
+  </si>
+  <si>
+    <t>https://attendee.gotowebinar.com/register/8281120664417331725</t>
+  </si>
+  <si>
+    <t>Have you ever wondered how to make an R Shiny app?  This webinar will show you how to make a Shiny app using a repeatable development pipeline provided by the R package golem.  The topics include how to set up the Shiny project, development of the Shiny app, and how to deploy the app locally.  The webinar will be most useful for intermediate to advanced R users although anyone interested in Shiny app development may find it interesting.</t>
+  </si>
+  <si>
+    <t>R shiny</t>
+  </si>
+  <si>
+    <t>https://attendee.gotowebinar.com/register/7582329347919390989</t>
+  </si>
+  <si>
+    <t>Building Shiny Apps</t>
   </si>
 </sst>
 </file>
@@ -242,7 +266,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/m/dd"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -254,6 +278,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -297,10 +329,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -320,8 +353,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -600,11 +637,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -751,16 +788,16 @@
         <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="I4" t="s">
         <v>25</v>
       </c>
       <c r="J4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="68" x14ac:dyDescent="0.2">
@@ -768,7 +805,7 @@
         <v>26</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="10">
         <v>43915</v>
@@ -783,19 +820,19 @@
         <v>29</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="I5" t="s">
         <v>25</v>
       </c>
       <c r="J5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="51" x14ac:dyDescent="0.2">
@@ -803,7 +840,7 @@
         <v>26</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="10">
         <v>43916</v>
@@ -818,19 +855,19 @@
         <v>29</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="I6" t="s">
         <v>25</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="51" x14ac:dyDescent="0.2">
@@ -838,7 +875,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="10">
         <v>43923</v>
@@ -853,19 +890,19 @@
         <v>29</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="I7" t="s">
         <v>25</v>
       </c>
       <c r="J7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="170" x14ac:dyDescent="0.2">
@@ -873,7 +910,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="10">
         <v>43917</v>
@@ -887,20 +924,20 @@
       <c r="F8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>46</v>
+      <c r="G8" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="H8" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="I8" t="s">
         <v>25</v>
       </c>
       <c r="J8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="68" x14ac:dyDescent="0.2">
@@ -908,7 +945,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="10">
         <v>43920</v>
@@ -923,19 +960,19 @@
         <v>29</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="I9" t="s">
         <v>25</v>
       </c>
       <c r="J9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -943,7 +980,7 @@
         <v>26</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="10">
         <v>43921</v>
@@ -958,19 +995,19 @@
         <v>29</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H10" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="I10" t="s">
         <v>25</v>
       </c>
       <c r="J10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="51" x14ac:dyDescent="0.2">
@@ -978,7 +1015,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C11" s="10">
         <v>43922</v>
@@ -993,57 +1030,131 @@
         <v>29</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H11" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="I11" t="s">
         <v>25</v>
       </c>
       <c r="J11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K11" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="K11" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C12" s="10">
-        <v>43923</v>
+        <v>43922</v>
       </c>
       <c r="D12" s="10">
-        <v>43923</v>
+        <v>43922</v>
       </c>
       <c r="E12">
-        <v>1585832400</v>
+        <v>1585746000</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>29</v>
       </c>
       <c r="G12" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" t="s">
         <v>62</v>
-      </c>
-      <c r="H12" t="s">
-        <v>30</v>
       </c>
       <c r="I12" t="s">
         <v>25</v>
       </c>
       <c r="J12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="10">
+        <v>43923</v>
+      </c>
+      <c r="D13" s="10">
+        <v>43923</v>
+      </c>
+      <c r="E13">
+        <v>1585832400</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" t="s">
+        <v>62</v>
+      </c>
+      <c r="I13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="K12" s="7" t="s">
-        <v>61</v>
+    </row>
+    <row r="14" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="10">
+        <v>43938</v>
+      </c>
+      <c r="D14" s="10">
+        <v>43938</v>
+      </c>
+      <c r="E14">
+        <v>1587117600</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G8" r:id="rId1" xr:uid="{B50FF027-3B2C-8445-8CFF-03561CE25368}"/>
+    <hyperlink ref="G13" r:id="rId2" xr:uid="{7BA32D85-CF7F-0A43-B242-3F19E213DBE2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
added covid-19 python semianrs
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/squiresrb/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D106E84-0D09-FC43-B5CA-94914B5F1933}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AD217C-4B34-724F-9BD9-5A0A644F6AD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="95">
   <si>
     <t>type</t>
   </si>
@@ -257,6 +257,78 @@
   </si>
   <si>
     <t>Building Shiny Apps</t>
+  </si>
+  <si>
+    <t>Introduction to Jupyter Notebooks and Anaconda</t>
+  </si>
+  <si>
+    <t>Project Jupyter is a open-source software project that supports interactive scientific computing with Python and R among many other languages. The Jupyter Lab is the main interface of the project, and the accompanying iPython kernel offers significance enhancements over the regular. We will explore Jupyter Lab and Jupyter Notebooks and learn how they can be used to perform cutting edge and reproducible data analysis, all the while enabling easy collaboration. This course is a prerequisite for the remainder of the Python Programming for Scientific seminars. Students will work in and receive Jupyter Notebooks with all lessons taught in the class for continued practice.</t>
+  </si>
+  <si>
+    <t>Introduction to Programming (for non-programmers)</t>
+  </si>
+  <si>
+    <t>If you have never programmed before, or if it has been a while, and you could use a refresher this is the seminar for you. We will explore why programming is important for scientists and how it can save time and enhance your science (though the rewards may not be obvious at first). We will learn the basic of the Python programming language as we walk through a preliminary analysis. Students will work in and receive Jupyter Notebooks with all lessons taught in the class for continued practice.</t>
+  </si>
+  <si>
+    <t>Python Programming for Scientists</t>
+  </si>
+  <si>
+    <t>Python is eating the world: How one developer's side project became the hottest programming language on the planet" is the title of an article from Aug 2019, and it echos the popularity of the Python programming language in general but also in science. In this seminar, we learn the python programming language as we iteratively build upon a temperature conversion project. Students will work in and receive Jupyter Notebooks with all lessons taught in the class for continued practice.</t>
+  </si>
+  <si>
+    <t>Data Analysis with Python and Pandas</t>
+  </si>
+  <si>
+    <t>Python is one of the most popular programming languages for data science. The pandas Python package is a primary reason for that popularity. In the seminar, we will utilize the pandas python package and apply it to the munging and analysis of a typical messy data set. Students will work in and receive Jupyter Notebooks with all lessons taught in the class for continued practice.</t>
+  </si>
+  <si>
+    <t>Data Visualization with Python</t>
+  </si>
+  <si>
+    <t>What is data without visualization? In this seminar, we will touch upon some data visualization guidelines and apply them in the most popular data visualization packages available in python for static and dynamic data visualization. Students will work in and receive Jupyter Notebooks with all lessons taught in the class for continued practice.</t>
+  </si>
+  <si>
+    <t>Intermediate Python Programming</t>
+  </si>
+  <si>
+    <t>Do you wish your Python programming was more "pythonic"? In the seminar, we will explore some advanced features of the Python programming language, and we will also explore some Python best practices. Students will work in and receive Jupyter Notebooks with all lessons taught in the class for continued practice.</t>
+  </si>
+  <si>
+    <t>Bioinformatics Programming with Python</t>
+  </si>
+  <si>
+    <t>Python is an ideal language for bioinformatics programming when one considers the general applicability of the language and the many bioinformatics-related packages that are readily available for it. In this seminar, we will explore some of the more relevant Python packages and delve into the bioconda project for easy bioinformatics software installation. Students will work in and receive Jupyter Notebooks with all lessons taught in the class for continued practice.</t>
+  </si>
+  <si>
+    <t>Building Workflows with Python</t>
+  </si>
+  <si>
+    <t>In this seminar, we will assemble a working pipeline based on the steps we have learned in the preceding seminars while surveying a few methods for building work flows, including the snakemake package. Students will work in and receive Jupyter Notebooks with all lessons taught in the class for continued practice.</t>
+  </si>
+  <si>
+    <t>Introduction to Machine Learning with Python and scikit-learn</t>
+  </si>
+  <si>
+    <t>Scikit-learn is a wildly popular Python package that enables you to quickly and easily create machine learning solutions to a host of problems. In this seminar, we will explore a number of the capabilities of the scikit-learn package, including classification, regression, clustering, dimensionality reduction and preprocessing. Students will work in and receive Jupyter Notebooks with all lessons taught in the class for continued practice.</t>
+  </si>
+  <si>
+    <t>Enabling Reproducible Science with Python and Jupyter</t>
+  </si>
+  <si>
+    <t>We will explore reasons for reproducible science and delve into practical exercises that will allow you to enhance your data analysis with good, better, and best practices. Topics include introduction to Jupyter Notebook, data and project organization, data exploration, automation, publishing, and sharing. This seminar will condense the Data Carpentry Reproducible Science Jupyter workshop held in Berkeley, CA in 2017 &amp; 2018 (https://github.com/Reproducible-Science-Curriculum). Students will receive a Jupyter Notebook with all steps taught in the class for further study and practice.</t>
+  </si>
+  <si>
+    <t>This webinar is the continuation of the previous webinar, Customizing Your Graphs using GraphPad Prism – Part I on 03/25. it will cover topics including changing and customizing graphs, visualization in descriptive statistics, basic survival analysis and curve fitting in GraphPad Prism. The webinar is intended for researchers with little to no experience using Prism 8, but almost everyone who uses Prism could benefit from this event</t>
+  </si>
+  <si>
+    <t>https://attendee.gotowebinar.com/register/5816582942988973325</t>
+  </si>
+  <si>
+    <t>jupyter, python, anaconda</t>
+  </si>
+  <si>
+    <t>python, programming</t>
   </si>
 </sst>
 </file>
@@ -637,11 +709,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="133" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1150,6 +1222,374 @@
         <v>68</v>
       </c>
     </row>
+    <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="10">
+        <v>43920</v>
+      </c>
+      <c r="D15" s="10">
+        <v>43920</v>
+      </c>
+      <c r="E15">
+        <v>1585591200</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H15" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" t="s">
+        <v>72</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="10">
+        <v>43922</v>
+      </c>
+      <c r="D16" s="10">
+        <v>43922</v>
+      </c>
+      <c r="E16">
+        <v>1585764000</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" t="s">
+        <v>74</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="10">
+        <v>43927</v>
+      </c>
+      <c r="D17" s="10">
+        <v>43927</v>
+      </c>
+      <c r="E17">
+        <v>1586196000</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" t="s">
+        <v>76</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="10">
+        <v>43929</v>
+      </c>
+      <c r="D18" s="10">
+        <v>43929</v>
+      </c>
+      <c r="E18">
+        <v>1586368800</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" t="s">
+        <v>62</v>
+      </c>
+      <c r="I18" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" t="s">
+        <v>78</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="10">
+        <v>43934</v>
+      </c>
+      <c r="D19" s="10">
+        <v>43934</v>
+      </c>
+      <c r="E19">
+        <v>1586800800</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" t="s">
+        <v>80</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="10">
+        <v>43936</v>
+      </c>
+      <c r="D20" s="10">
+        <v>43936</v>
+      </c>
+      <c r="E20">
+        <v>1586973600</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H20" t="s">
+        <v>62</v>
+      </c>
+      <c r="I20" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" t="s">
+        <v>82</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="10">
+        <v>43941</v>
+      </c>
+      <c r="D21" s="10">
+        <v>43941</v>
+      </c>
+      <c r="E21">
+        <v>1587405600</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" t="s">
+        <v>25</v>
+      </c>
+      <c r="J21" t="s">
+        <v>84</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="10">
+        <v>43943</v>
+      </c>
+      <c r="D22" s="10">
+        <v>43943</v>
+      </c>
+      <c r="E22">
+        <v>1587578400</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" t="s">
+        <v>86</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="10">
+        <v>43948</v>
+      </c>
+      <c r="D23" s="10">
+        <v>43948</v>
+      </c>
+      <c r="E23">
+        <v>1588010400</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H23" t="s">
+        <v>62</v>
+      </c>
+      <c r="I23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" t="s">
+        <v>88</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="10">
+        <v>43950</v>
+      </c>
+      <c r="D24" s="10">
+        <v>43950</v>
+      </c>
+      <c r="E24">
+        <v>1588183200</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" t="s">
+        <v>62</v>
+      </c>
+      <c r="I24" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" t="s">
+        <v>90</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="B25"/>
+      <c r="G25" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H25" t="s">
+        <v>62</v>
+      </c>
+      <c r="I25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" t="s">
+        <v>91</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G8" r:id="rId1" xr:uid="{B50FF027-3B2C-8445-8CFF-03561CE25368}"/>

</xml_diff>

<commit_message>
Added phylogenetic and Part 2 of Prism series
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/squiresrb/Documents/GitHub/nbp_events_niaid/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AD217C-4B34-724F-9BD9-5A0A644F6AD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2752D759-633A-1048-B387-F2E895E6D4EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13780" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="102">
   <si>
     <t>type</t>
   </si>
@@ -319,9 +319,6 @@
     <t>We will explore reasons for reproducible science and delve into practical exercises that will allow you to enhance your data analysis with good, better, and best practices. Topics include introduction to Jupyter Notebook, data and project organization, data exploration, automation, publishing, and sharing. This seminar will condense the Data Carpentry Reproducible Science Jupyter workshop held in Berkeley, CA in 2017 &amp; 2018 (https://github.com/Reproducible-Science-Curriculum). Students will receive a Jupyter Notebook with all steps taught in the class for further study and practice.</t>
   </si>
   <si>
-    <t>This webinar is the continuation of the previous webinar, Customizing Your Graphs using GraphPad Prism – Part I on 03/25. it will cover topics including changing and customizing graphs, visualization in descriptive statistics, basic survival analysis and curve fitting in GraphPad Prism. The webinar is intended for researchers with little to no experience using Prism 8, but almost everyone who uses Prism could benefit from this event</t>
-  </si>
-  <si>
     <t>https://attendee.gotowebinar.com/register/5816582942988973325</t>
   </si>
   <si>
@@ -329,6 +326,30 @@
   </si>
   <si>
     <t>python, programming</t>
+  </si>
+  <si>
+    <t>https://attendee.gotowebinar.com/register/550899711803711757</t>
+  </si>
+  <si>
+    <t>This online demo will provide an introduction to the MEGAX software package. The session will take the user from the initial step of using a GenBank ID to pull homologous sequences out of the database, through the process of generating a high-quality multiple sequence alignment with the downloaded data, to the final step of calculating a phylogenetic tree with the aligned sequences.</t>
+  </si>
+  <si>
+    <t>phylogenetics,GenBank,MEGAX</t>
+  </si>
+  <si>
+    <t>From a GenBank ID to a Phylogenetic Tree in MEGAX</t>
+  </si>
+  <si>
+    <t>Customizing Your Graphs using GraphPad Prism 8 - Part II</t>
+  </si>
+  <si>
+    <t>Prism,statistics</t>
+  </si>
+  <si>
+    <t>This webinar is the continuation of the previous webinar, Customizing Your Graphs using GraphPad Prism – Part I on 03/25. it will cover topics including changing and customizing graphs, visualization in descriptive statistics, basic survival analysis and curve fitting in GraphPad Prism. The webinar is intended for researchers with little to no experience using Prism 8, but almost everyone who uses Prism could benefit from this event.</t>
+  </si>
+  <si>
+    <t>https://attendee.gotowebinar.com/register/1426715698908901901</t>
   </si>
 </sst>
 </file>
@@ -709,11 +730,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="133" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1206,7 +1227,7 @@
       <c r="F14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H14" t="s">
@@ -1222,7 +1243,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1241,23 +1262,23 @@
       <c r="F15" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H15" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="K15" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="H15" t="s">
-        <v>62</v>
-      </c>
-      <c r="I15" t="s">
-        <v>25</v>
-      </c>
-      <c r="J15" t="s">
-        <v>72</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1277,7 +1298,7 @@
         <v>29</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H16" t="s">
         <v>62</v>
@@ -1285,14 +1306,14 @@
       <c r="I16" t="s">
         <v>25</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="7" t="s">
         <v>74</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1312,7 +1333,7 @@
         <v>29</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H17" t="s">
         <v>62</v>
@@ -1320,14 +1341,14 @@
       <c r="I17" t="s">
         <v>25</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="7" t="s">
         <v>76</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1347,7 +1368,7 @@
         <v>29</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H18" t="s">
         <v>62</v>
@@ -1355,14 +1376,14 @@
       <c r="I18" t="s">
         <v>25</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="7" t="s">
         <v>78</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1382,7 +1403,7 @@
         <v>29</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H19" t="s">
         <v>62</v>
@@ -1390,14 +1411,14 @@
       <c r="I19" t="s">
         <v>25</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="7" t="s">
         <v>80</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1417,7 +1438,7 @@
         <v>29</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H20" t="s">
         <v>62</v>
@@ -1425,14 +1446,14 @@
       <c r="I20" t="s">
         <v>25</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="7" t="s">
         <v>82</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1452,7 +1473,7 @@
         <v>29</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H21" t="s">
         <v>62</v>
@@ -1460,14 +1481,14 @@
       <c r="I21" t="s">
         <v>25</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="7" t="s">
         <v>84</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1487,7 +1508,7 @@
         <v>29</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H22" t="s">
         <v>62</v>
@@ -1495,14 +1516,14 @@
       <c r="I22" t="s">
         <v>25</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="7" t="s">
         <v>86</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1522,7 +1543,7 @@
         <v>29</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H23" t="s">
         <v>62</v>
@@ -1530,14 +1551,14 @@
       <c r="I23" t="s">
         <v>25</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="7" t="s">
         <v>88</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1557,7 +1578,7 @@
         <v>29</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H24" t="s">
         <v>62</v>
@@ -1565,35 +1586,90 @@
       <c r="I24" t="s">
         <v>25</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="7" t="s">
         <v>90</v>
       </c>
       <c r="K24" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="10">
+        <v>43930</v>
+      </c>
+      <c r="D25" s="10">
+        <v>43930</v>
+      </c>
+      <c r="E25">
+        <v>1586426400</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="7" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="B25"/>
-      <c r="G25" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="H25" t="s">
         <v>62</v>
       </c>
       <c r="I25" t="s">
         <v>25</v>
       </c>
-      <c r="J25" t="s">
-        <v>91</v>
+      <c r="J25" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="10">
+        <v>43931</v>
+      </c>
+      <c r="D26" s="10">
+        <v>43931</v>
+      </c>
+      <c r="E26">
+        <v>1586512800</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="H26" t="s">
+        <v>62</v>
+      </c>
+      <c r="I26" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G8" r:id="rId1" xr:uid="{B50FF027-3B2C-8445-8CFF-03561CE25368}"/>
     <hyperlink ref="G13" r:id="rId2" xr:uid="{7BA32D85-CF7F-0A43-B242-3F19E213DBE2}"/>
+    <hyperlink ref="G26" r:id="rId3" xr:uid="{3F296552-766E-8F4D-B9EC-322368070C73}"/>
+    <hyperlink ref="G14" r:id="rId4" xr:uid="{DF842FBF-8CD0-744A-8819-20706BA11B2E}"/>
+    <hyperlink ref="G15" r:id="rId5" xr:uid="{DFEC78E2-A5CA-3146-8AC1-A7A8E3368DD7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
removed duplicate python events
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/squiresrb/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{503A2966-66C8-F640-8D9D-4C3213DD8856}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DADB136-E7AA-8D4A-9DB8-B63849DBBC4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
   <si>
     <t>type</t>
   </si>
@@ -153,60 +153,6 @@
     <t>Building Shiny Apps</t>
   </si>
   <si>
-    <t>Python Programming for Scientists</t>
-  </si>
-  <si>
-    <t>Python is eating the world: How one developer's side project became the hottest programming language on the planet" is the title of an article from Aug 2019, and it echos the popularity of the Python programming language in general but also in science. In this seminar, we learn the python programming language as we iteratively build upon a temperature conversion project. Students will work in and receive Jupyter Notebooks with all lessons taught in the class for continued practice.</t>
-  </si>
-  <si>
-    <t>Data Analysis with Python and Pandas</t>
-  </si>
-  <si>
-    <t>Python is one of the most popular programming languages for data science. The pandas Python package is a primary reason for that popularity. In the seminar, we will utilize the pandas python package and apply it to the munging and analysis of a typical messy data set. Students will work in and receive Jupyter Notebooks with all lessons taught in the class for continued practice.</t>
-  </si>
-  <si>
-    <t>Data Visualization with Python</t>
-  </si>
-  <si>
-    <t>What is data without visualization? In this seminar, we will touch upon some data visualization guidelines and apply them in the most popular data visualization packages available in python for static and dynamic data visualization. Students will work in and receive Jupyter Notebooks with all lessons taught in the class for continued practice.</t>
-  </si>
-  <si>
-    <t>Intermediate Python Programming</t>
-  </si>
-  <si>
-    <t>Do you wish your Python programming was more "pythonic"? In the seminar, we will explore some advanced features of the Python programming language, and we will also explore some Python best practices. Students will work in and receive Jupyter Notebooks with all lessons taught in the class for continued practice.</t>
-  </si>
-  <si>
-    <t>Bioinformatics Programming with Python</t>
-  </si>
-  <si>
-    <t>Python is an ideal language for bioinformatics programming when one considers the general applicability of the language and the many bioinformatics-related packages that are readily available for it. In this seminar, we will explore some of the more relevant Python packages and delve into the bioconda project for easy bioinformatics software installation. Students will work in and receive Jupyter Notebooks with all lessons taught in the class for continued practice.</t>
-  </si>
-  <si>
-    <t>Building Workflows with Python</t>
-  </si>
-  <si>
-    <t>In this seminar, we will assemble a working pipeline based on the steps we have learned in the preceding seminars while surveying a few methods for building work flows, including the snakemake package. Students will work in and receive Jupyter Notebooks with all lessons taught in the class for continued practice.</t>
-  </si>
-  <si>
-    <t>Introduction to Machine Learning with Python and scikit-learn</t>
-  </si>
-  <si>
-    <t>Scikit-learn is a wildly popular Python package that enables you to quickly and easily create machine learning solutions to a host of problems. In this seminar, we will explore a number of the capabilities of the scikit-learn package, including classification, regression, clustering, dimensionality reduction and preprocessing. Students will work in and receive Jupyter Notebooks with all lessons taught in the class for continued practice.</t>
-  </si>
-  <si>
-    <t>Enabling Reproducible Science with Python and Jupyter</t>
-  </si>
-  <si>
-    <t>We will explore reasons for reproducible science and delve into practical exercises that will allow you to enhance your data analysis with good, better, and best practices. Topics include introduction to Jupyter Notebook, data and project organization, data exploration, automation, publishing, and sharing. This seminar will condense the Data Carpentry Reproducible Science Jupyter workshop held in Berkeley, CA in 2017 &amp; 2018 (https://github.com/Reproducible-Science-Curriculum). Students will receive a Jupyter Notebook with all steps taught in the class for further study and practice.</t>
-  </si>
-  <si>
-    <t>https://attendee.gotowebinar.com/register/5816582942988973325</t>
-  </si>
-  <si>
-    <t>python, programming</t>
-  </si>
-  <si>
     <t>https://attendee.gotowebinar.com/register/550899711803711757</t>
   </si>
   <si>
@@ -262,9 +208,6 @@
   </si>
   <si>
     <t>GoToWebinar (10:00 – 11:00 am)</t>
-  </si>
-  <si>
-    <t>GoToWebinar (2:00 – 4:00 pm)</t>
   </si>
 </sst>
 </file>
@@ -645,11 +588,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -790,7 +733,7 @@
         <v>1585832400</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>30</v>
@@ -825,7 +768,7 @@
         <v>1587117600</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>34</v>
@@ -843,27 +786,27 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
       <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="10">
+        <v>43930</v>
+      </c>
+      <c r="D6" s="10">
+        <v>43930</v>
+      </c>
+      <c r="E6">
+        <v>1586426400</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="C6" s="10">
-        <v>43927</v>
-      </c>
-      <c r="D6" s="10">
-        <v>43927</v>
-      </c>
-      <c r="E6">
-        <v>1586196000</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="H6" t="s">
         <v>31</v>
@@ -871,34 +814,34 @@
       <c r="I6" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="3" t="s">
         <v>37</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
-        <v>38</v>
+      <c r="B7" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="C7" s="10">
-        <v>43929</v>
+        <v>43931</v>
       </c>
       <c r="D7" s="10">
-        <v>43929</v>
+        <v>43931</v>
       </c>
       <c r="E7">
-        <v>1586368800</v>
+        <v>1586512800</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -906,34 +849,34 @@
       <c r="I7" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="7" t="s">
-        <v>39</v>
+      <c r="J7" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>40</v>
+      <c r="B8" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="C8" s="10">
-        <v>43934</v>
+        <v>43937</v>
       </c>
       <c r="D8" s="10">
-        <v>43934</v>
+        <v>43937</v>
       </c>
       <c r="E8">
-        <v>1586800800</v>
+        <v>1587031200</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H8" t="s">
         <v>31</v>
@@ -941,34 +884,34 @@
       <c r="I8" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="7" t="s">
-        <v>41</v>
+      <c r="J8" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
-        <v>42</v>
+      <c r="B9" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="C9" s="10">
-        <v>43936</v>
+        <v>43924</v>
       </c>
       <c r="D9" s="10">
-        <v>43936</v>
+        <v>43924</v>
       </c>
       <c r="E9">
-        <v>1586973600</v>
+        <v>1585908000</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
         <v>31</v>
@@ -976,297 +919,17 @@
       <c r="I9" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="7" t="s">
-        <v>43</v>
+      <c r="J9" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="68" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="10">
-        <v>43941</v>
-      </c>
-      <c r="D10" s="10">
-        <v>43941</v>
-      </c>
-      <c r="E10">
-        <v>1587405600</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="10">
-        <v>43943</v>
-      </c>
-      <c r="D11" s="10">
-        <v>43943</v>
-      </c>
-      <c r="E11">
-        <v>1587578400</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H11" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="68" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="10">
-        <v>43948</v>
-      </c>
-      <c r="D12" s="10">
-        <v>43948</v>
-      </c>
-      <c r="E12">
-        <v>1588010400</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" t="s">
-        <v>31</v>
-      </c>
-      <c r="I12" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="85" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="10">
-        <v>43950</v>
-      </c>
-      <c r="D13" s="10">
-        <v>43950</v>
-      </c>
-      <c r="E13">
-        <v>1588183200</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" t="s">
-        <v>25</v>
-      </c>
-      <c r="J13" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="68" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="10">
-        <v>43930</v>
-      </c>
-      <c r="D14" s="10">
-        <v>43930</v>
-      </c>
-      <c r="E14">
-        <v>1586426400</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" t="s">
-        <v>31</v>
-      </c>
-      <c r="I14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="68" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="10">
-        <v>43931</v>
-      </c>
-      <c r="D15" s="10">
-        <v>43931</v>
-      </c>
-      <c r="E15">
-        <v>1586512800</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="H15" t="s">
-        <v>31</v>
-      </c>
-      <c r="I15" t="s">
-        <v>25</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="10">
-        <v>43937</v>
-      </c>
-      <c r="D16" s="10">
-        <v>43937</v>
-      </c>
-      <c r="E16">
-        <v>1587031200</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" t="s">
-        <v>25</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="10">
-        <v>43924</v>
-      </c>
-      <c r="D17" s="10">
-        <v>43924</v>
-      </c>
-      <c r="E17">
-        <v>1585908000</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H17" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" xr:uid="{7BA32D85-CF7F-0A43-B242-3F19E213DBE2}"/>
-    <hyperlink ref="G15" r:id="rId2" xr:uid="{3F296552-766E-8F4D-B9EC-322368070C73}"/>
+    <hyperlink ref="G7" r:id="rId2" xr:uid="{3F296552-766E-8F4D-B9EC-322368070C73}"/>
     <hyperlink ref="G5" r:id="rId3" xr:uid="{DF842FBF-8CD0-744A-8819-20706BA11B2E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Nephele webinar to schedule
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/squiresrb/Documents/GitHub/nbp_events_niaid/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DADB136-E7AA-8D4A-9DB8-B63849DBBC4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE83C2AA-2A67-EC4A-9C05-D4EC4E7F8E44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8380" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>type</t>
   </si>
@@ -126,18 +126,6 @@
     <t>NIAID BioIT listserv</t>
   </si>
   <si>
-    <t>Preparing and Submitting Protein Structures to the NIAID 3D Printing Service</t>
-  </si>
-  <si>
-    <t>This webinar will demonstrate the procedures for creating protein structure visualizations using UCSF Chimera, and the considerations for efficiently submitting them to the NIAID 3D printing service provided by the Bioinformatics and Computational Biosciences Branch (BCBB).  Use of the NIH 3D Print Exchange to generate models will also be discussed: https://3dprint.nih.gov. Note that 3D printing is a free service provided to NIAID to further the mission of the Institute.  Chimera software is available from https://www.cgl.ucsf.edu/chimera/download.html.</t>
-  </si>
-  <si>
-    <t>Chimera,3D print,models</t>
-  </si>
-  <si>
-    <t>https://attendee.gotowebinar.com/register/2509636795587133709</t>
-  </si>
-  <si>
     <t>Webinar</t>
   </si>
   <si>
@@ -153,30 +141,6 @@
     <t>Building Shiny Apps</t>
   </si>
   <si>
-    <t>https://attendee.gotowebinar.com/register/550899711803711757</t>
-  </si>
-  <si>
-    <t>This online demo will provide an introduction to the MEGAX software package. The session will take the user from the initial step of using a GenBank ID to pull homologous sequences out of the database, through the process of generating a high-quality multiple sequence alignment with the downloaded data, to the final step of calculating a phylogenetic tree with the aligned sequences.</t>
-  </si>
-  <si>
-    <t>phylogenetics,GenBank,MEGAX</t>
-  </si>
-  <si>
-    <t>From a GenBank ID to a Phylogenetic Tree in MEGAX</t>
-  </si>
-  <si>
-    <t>Customizing Your Graphs using GraphPad Prism 8 - Part II</t>
-  </si>
-  <si>
-    <t>Prism,statistics</t>
-  </si>
-  <si>
-    <t>This webinar is the continuation of the previous webinar, Customizing Your Graphs using GraphPad Prism – Part I on 03/25. it will cover topics including changing and customizing graphs, visualization in descriptive statistics, basic survival analysis and curve fitting in GraphPad Prism. The webinar is intended for researchers with little to no experience using Prism 8, but almost everyone who uses Prism could benefit from this event.</t>
-  </si>
-  <si>
-    <t>https://attendee.gotowebinar.com/register/1426715698908901901</t>
-  </si>
-  <si>
     <t>https://attendee.gotowebinar.com/register/6558548782752896782</t>
   </si>
   <si>
@@ -189,25 +153,22 @@
     <t>Molecular Visualization with Chimera - Part II</t>
   </si>
   <si>
-    <t xml:space="preserve">Introducation to UNIX - Part II </t>
-  </si>
-  <si>
-    <t>https://attendee.gotowebinar.com/register/1900531543287311374</t>
-  </si>
-  <si>
-    <t>The raw output of biological research is usually in the form of large text files. UNIX is particularly suited to working with such files and has several powerful and flexible commands that can process such data. In UNIX, user types everything and it may seem archaic to use a keyboard to issue commands. However, it’s much easier to automate keyboard tasks than mouse tasks and this course is a gentle introduction on how UNIX commands can be combined and automated to handle biological data.</t>
-  </si>
-  <si>
-    <t>UNIX</t>
-  </si>
-  <si>
-    <t>GoToWebinar (10:00 am – 12:00 pm)</t>
-  </si>
-  <si>
-    <t>GoToWebinar (1:00 – 2:00 pm)</t>
-  </si>
-  <si>
     <t>GoToWebinar (10:00 – 11:00 am)</t>
+  </si>
+  <si>
+    <t>Studying the Microbiome Using the Nephele Web Platform</t>
+  </si>
+  <si>
+    <t>GoToWebinar (1:00 – 2:00 pm))</t>
+  </si>
+  <si>
+    <t>https://attendee.gotowebinar.com/register/4895163611488872973</t>
+  </si>
+  <si>
+    <t>This webinar will demonstrate how to process and analyze a 16S microbiome dataset as well as a shotgun metagenomics dataset using the pipelines available in the Nephele platform.</t>
+  </si>
+  <si>
+    <t>microbiome,analysis,cloud computing</t>
   </si>
 </sst>
 </file>
@@ -588,11 +549,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -716,30 +677,30 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C4" s="10">
-        <v>43923</v>
+        <v>43938</v>
       </c>
       <c r="D4" s="10">
-        <v>43923</v>
+        <v>43938</v>
       </c>
       <c r="E4">
-        <v>1585832400</v>
+        <v>1587117600</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I4" t="s">
         <v>25</v>
@@ -751,7 +712,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -759,178 +720,72 @@
         <v>35</v>
       </c>
       <c r="C5" s="10">
-        <v>43938</v>
+        <v>43937</v>
       </c>
       <c r="D5" s="10">
-        <v>43938</v>
+        <v>43937</v>
       </c>
       <c r="E5">
-        <v>1587117600</v>
+        <v>1587031200</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I5" t="s">
         <v>25</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="10">
+        <v>43942</v>
+      </c>
+      <c r="D6" s="10">
+        <v>43942</v>
+      </c>
+      <c r="E6">
+        <v>1587474000</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="10">
-        <v>43930</v>
-      </c>
-      <c r="D6" s="10">
-        <v>43930</v>
-      </c>
-      <c r="E6">
-        <v>1586426400</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>36</v>
-      </c>
       <c r="H6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I6" t="s">
         <v>25</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="68" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="10">
-        <v>43931</v>
-      </c>
-      <c r="D7" s="10">
-        <v>43931</v>
-      </c>
-      <c r="E7">
-        <v>1586512800</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K7" s="7" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="10">
-        <v>43937</v>
-      </c>
-      <c r="D8" s="10">
-        <v>43937</v>
-      </c>
-      <c r="E8">
-        <v>1587031200</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="85" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="10">
-        <v>43924</v>
-      </c>
-      <c r="D9" s="10">
-        <v>43924</v>
-      </c>
-      <c r="E9">
-        <v>1585908000</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G4" r:id="rId1" xr:uid="{7BA32D85-CF7F-0A43-B242-3F19E213DBE2}"/>
-    <hyperlink ref="G7" r:id="rId2" xr:uid="{3F296552-766E-8F4D-B9EC-322368070C73}"/>
-    <hyperlink ref="G5" r:id="rId3" xr:uid="{DF842FBF-8CD0-744A-8819-20706BA11B2E}"/>
+    <hyperlink ref="G4" r:id="rId1" xr:uid="{DF842FBF-8CD0-744A-8819-20706BA11B2E}"/>
+    <hyperlink ref="G6" r:id="rId2" xr:uid="{A4E509AB-FF2E-6E43-B4D1-AB8CC4AE1A56}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Updated with TYCTW day link
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/booirizarryy/Documents/nbp_events_niaid/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipskm2/Documents/GitHub/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3D01C1-C597-C047-97B5-7A03CFE6C9B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CB9363-6A27-D64D-8D88-A90C3D04A9A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4160" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>type</t>
   </si>
@@ -73,6 +73,45 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Virtual Event</t>
+  </si>
+  <si>
+    <t>https://bioinformatics.niaid.nih.gov/take-your-child-to-work</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>The NIH Office of Research Services hosts the annual Take Your Child to Work Day with an aim to inspire the next generation of NIH daughters and sons in grades 1-12 to explore career paths in science and public service at our nation’s medical research agency. 2021 is being held as a virtual event. Registration has closed, but resources provided by NIAID’s 3D Printing and Biovisualization Program are being made publicly available here.</t>
+  </si>
+  <si>
+    <t>3D,visualization,STEM</t>
+  </si>
+  <si>
+    <t>2021 Take Your Child to Work Day</t>
+  </si>
+  <si>
+    <t>NIH ALL STAFF LISTSERV</t>
+  </si>
+  <si>
+    <t>STRUCTBIOLIG LISTSERV</t>
+  </si>
+  <si>
+    <t>Advances in COVID-19 Prevention and Treatment Enabled by Structural Biology Research</t>
+  </si>
+  <si>
+    <t>Virtual Workshop</t>
+  </si>
+  <si>
+    <t>https://www.aps.anl.gov/sites/www.aps.anl.gov/files/APS-Uploads/WK9%20Agenda.pdf</t>
+  </si>
+  <si>
+    <t>Broadly, the workshop will present areas where structural biology research, including macromolecular crystallography and cryoelectron microscopy, intersects with in vivo, in vitro, and in silico studies of SARS-CoV-2 and COVID-19. More precisely, the topics will include (a) viral biology, (b) vaccine, therapeutic, and diagnostic antibody studies, and (c) small-molecule drug discovery as it relates to viral proteases and other viral proteins. In addition, as this year's events emphasize the need for a coordinated, long-term strategy to prevent future pandemics of zoonotic origin, a broader One Health perspective on viral pathogens will be presented.</t>
+  </si>
+  <si>
+    <t>structural biology,crystallography,SARS-CoV-2,drug discovery</t>
   </si>
 </sst>
 </file>
@@ -439,11 +478,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="4" sqref="A6:XFD6 A2:XFD2 A3:XFD3 A4:XFD4 A5:XFD5"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -454,6 +493,7 @@
     <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="89.1640625" style="7" customWidth="1"/>
     <col min="7" max="7" width="70.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="104.33203125" style="3" customWidth="1"/>
     <col min="11" max="11" width="28.33203125" style="7" customWidth="1"/>
     <col min="12" max="12" width="49.33203125" style="5" customWidth="1"/>
@@ -497,6 +537,76 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="9">
+        <v>44308</v>
+      </c>
+      <c r="D2" s="9">
+        <v>44308</v>
+      </c>
+      <c r="E2">
+        <v>1619096400</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="9">
+        <v>44327</v>
+      </c>
+      <c r="D3" s="9">
+        <v>44328</v>
+      </c>
+      <c r="E3">
+        <v>1620741600</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
add new csv file for testing
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/booirizarryy/Documents/nbp_events_niaid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF070645-7EF7-0442-B8DF-F769FD4C5A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E959BF4A-C775-6E4B-A939-DC976D084C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-280" yWindow="-18940" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3720" yWindow="-18940" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="25">
   <si>
     <t>type</t>
   </si>
@@ -97,6 +97,21 @@
   </si>
   <si>
     <t>https://bioinformatics.niaid.nih.gov/rsna-2023</t>
+  </si>
+  <si>
+    <t>RSNA-2 2023</t>
+  </si>
+  <si>
+    <t>RSNA -3 2023</t>
+  </si>
+  <si>
+    <t>RSNA- 4 2023</t>
+  </si>
+  <si>
+    <t>RSNA -5 2023</t>
+  </si>
+  <si>
+    <t>RSNA - 6 2023</t>
   </si>
 </sst>
 </file>
@@ -180,7 +195,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -199,9 +214,6 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -487,11 +499,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -559,13 +571,13 @@
       <c r="D2" s="9">
         <v>45259</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="11">
         <v>1700956851</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>19</v>
       </c>
       <c r="H2" t="s">
@@ -574,16 +586,196 @@
       <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="7" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="9">
+        <v>45256</v>
+      </c>
+      <c r="D3" s="9">
+        <v>45259</v>
+      </c>
+      <c r="E3" s="11">
+        <v>1700956851</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="9">
+        <v>45256</v>
+      </c>
+      <c r="D4" s="9">
+        <v>45259</v>
+      </c>
+      <c r="E4" s="11">
+        <v>1700956851</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="9">
+        <v>45256</v>
+      </c>
+      <c r="D5" s="9">
+        <v>45259</v>
+      </c>
+      <c r="E5" s="11">
+        <v>1700956851</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="9">
+        <v>45256</v>
+      </c>
+      <c r="D6" s="9">
+        <v>45259</v>
+      </c>
+      <c r="E6" s="11">
+        <v>1700956851</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="9">
+        <v>45256</v>
+      </c>
+      <c r="D7" s="9">
+        <v>45259</v>
+      </c>
+      <c r="E7" s="11">
+        <v>1700956851</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="7" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{C9A4FCE5-4417-2945-BA19-63E1359A3180}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{905398DB-FC2D-214A-836D-560FE28E7DD4}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{05917AEF-A05D-9945-BBCC-06C89438AEE7}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{D5FDA7F8-91B4-F94C-A6E3-7C2B98F51580}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{AEFC40F6-350B-4D4E-84F2-B819B65D214B}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{3F09E39B-BC98-DC47-BE7E-3354FBF84790}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>